<commit_message>
added test cases for data extraction
git-svn-id: svn://localhost/ARK/trunk@8111 35ee9b83-dd2c-47f4-99a2-c706670c48ce
</commit_message>
<xml_diff>
--- a/usefulTools/UAT_FutureRequests.xlsx
+++ b/usefulTools/UAT_FutureRequests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="497">
   <si>
     <t>Result coding: 1 = Pass (full functionality with no unexpected errors), 0 = Fail (lack of required functionality or reproducible error during testing), 9 = Conditional (partial functionality, error during testing which cannot be reproduced, poor user experience or other constraints) X = Functionality which is desirable for future iterations of the system. these items are not necessary for user acceptance of this version of the system</t>
   </si>
@@ -1059,6 +1059,9 @@
     <t>A user with sufficient access can search data for all fields for a subject.</t>
   </si>
   <si>
+    <t>this is expanded below to include all the fields and ensure testing covers all </t>
+  </si>
+  <si>
     <t>1. The user is able to search for certain results entered in any number of the relevant fields.</t>
   </si>
   <si>
@@ -1066,6 +1069,258 @@
   </si>
   <si>
     <t>if we enter it, we want to be able to search it - lisa's catchphrase.  We will analyse and test this for the next realease when Data Extraction is due</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "First Name"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Consent Date"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Subject UID"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Post Code"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Last Name"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Sex"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Vital Status"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Marital Status"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "DOB"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Date of Death"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Cause of Death"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Preferred Email"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Other Email"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Last Known Alive"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Building Name/Unit"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Street Address"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "City"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Country"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "State"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Other State"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Address Status"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Address Type"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Phone Number"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Title"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Contact Method"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Status"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Consent Status"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Consent Type"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Consent Downloaded"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Consent To Passive Data Gathering"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Consent To Active Contact"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Consent To Use Data"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Heard About Study"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Subject Comments"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Other Email Status"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "PreferredEmailStatus"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Date Address Received"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Address Comments"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Address Source"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Phone Type"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Area Code"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Phone Status"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Phone Source"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Date Received"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Silent Mode"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Phone Comment"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "First Name"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Consent Date"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Subject UID"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Post Code"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Last Name"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Sex"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Vital Status"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Marital Status"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "DOB"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Date of Death"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Cause of Death"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Preferred Email"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Other Email"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Last Known Alive"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Building Name/Unit"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Street Address"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "City"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Country"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "State"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Other State"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Address Status"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Address Type"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Title"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Contact Method"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Status"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Consent Status"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Consent Type"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Consent Downloaded"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Consent To Passive Data Gathering"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Consent To Active Contact"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Consent To Use Data"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Heard About Study"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Subject Comments"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Other Email Status"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "PreferredEmailStatus"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Date Address Received"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Address Comments"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Address Source"</t>
   </si>
   <si>
     <t>A user with sufficient access can search data for all custom fields entered against a subject.</t>
@@ -1460,7 +1715,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="69">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
@@ -1685,6 +1940,13 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="2" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
@@ -1774,29 +2036,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R225"/>
+  <dimension ref="A1:R323"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A43" view="normal" windowProtection="false" workbookViewId="0" zoomScale="54" zoomScaleNormal="54" zoomScalePageLayoutView="100">
-      <selection activeCell="A51" activeCellId="0" pane="topLeft" sqref="A51"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A265" view="normal" windowProtection="false" workbookViewId="0" zoomScale="54" zoomScaleNormal="54" zoomScalePageLayoutView="100">
+      <selection activeCell="B272" activeCellId="0" pane="topLeft" sqref="B272"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.49019607843137"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="34.1254901960784"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="44.0509803921569"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="40.3058823529412"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="33.8745098039216"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="8.89803921568628"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="1.91372549019608"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="6.35294117647059"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="37.1254901960784"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="4" width="8.89803921568628"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="4" width="17.6470588235294"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="6.35294117647059"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="6" width="37.1254901960784"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.2039215686275"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="8.68235294117647"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="7" width="9.64313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.51764705882353"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="34.2705882352941"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="44.2352941176471"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="40.4705882352941"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="34.0117647058824"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="8.93333333333333"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="1.92156862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="6.38039215686275"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="6" width="37.2823529411765"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="4" width="8.93333333333333"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="4" width="17.7176470588235"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="6.38039215686275"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="6" width="37.2823529411765"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.2666666666667"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="8.72156862745098"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="7" width="9.68235294117647"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="68.95" outlineLevel="0" r="1">
@@ -6509,13 +6771,13 @@
         <v>346</v>
       </c>
       <c r="C182" s="31" t="s">
-        <v>22</v>
+        <v>347</v>
       </c>
       <c r="D182" s="32" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E182" s="32" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="F182" s="16"/>
       <c r="G182" s="16"/>
@@ -6527,318 +6789,208 @@
         <v>33</v>
       </c>
       <c r="M182" s="19" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.5" outlineLevel="0" r="183">
-      <c r="B183" s="30" t="s">
         <v>350</v>
       </c>
-      <c r="C183" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D183" s="32" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="183">
+      <c r="B183" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="E183" s="32" t="s">
-        <v>352</v>
-      </c>
+      <c r="C183" s="31"/>
+      <c r="D183" s="32"/>
+      <c r="E183" s="32"/>
       <c r="F183" s="16"/>
       <c r="G183" s="16"/>
       <c r="H183" s="18"/>
       <c r="I183" s="19"/>
       <c r="J183" s="16"/>
       <c r="K183" s="16"/>
-      <c r="L183" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M183" s="19" t="s">
-        <v>349</v>
-      </c>
+      <c r="L183" s="18"/>
+      <c r="M183" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="184">
-      <c r="B184" s="30" t="s">
-        <v>353</v>
-      </c>
-      <c r="C184" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D184" s="32" t="s">
-        <v>347</v>
-      </c>
-      <c r="E184" s="32" t="s">
-        <v>348</v>
-      </c>
+      <c r="B184" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="C184" s="31"/>
+      <c r="D184" s="32"/>
+      <c r="E184" s="32"/>
       <c r="F184" s="16"/>
       <c r="G184" s="16"/>
       <c r="H184" s="18"/>
       <c r="I184" s="19"/>
       <c r="J184" s="16"/>
       <c r="K184" s="16"/>
-      <c r="L184" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M184" s="19" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.5" outlineLevel="0" r="185">
-      <c r="B185" s="30" t="s">
-        <v>354</v>
-      </c>
-      <c r="C185" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D185" s="32" t="s">
-        <v>351</v>
-      </c>
-      <c r="E185" s="32" t="s">
-        <v>352</v>
-      </c>
+      <c r="L184" s="18"/>
+      <c r="M184" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="185">
+      <c r="B185" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="C185" s="31"/>
+      <c r="D185" s="32"/>
+      <c r="E185" s="32"/>
       <c r="F185" s="16"/>
       <c r="G185" s="16"/>
       <c r="H185" s="18"/>
       <c r="I185" s="19"/>
       <c r="J185" s="16"/>
       <c r="K185" s="16"/>
-      <c r="L185" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M185" s="19" t="s">
-        <v>349</v>
-      </c>
+      <c r="L185" s="18"/>
+      <c r="M185" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="186">
-      <c r="B186" s="30" t="s">
-        <v>355</v>
-      </c>
-      <c r="C186" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D186" s="32" t="s">
-        <v>347</v>
-      </c>
-      <c r="E186" s="32" t="s">
-        <v>348</v>
-      </c>
+      <c r="B186" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="C186" s="31"/>
+      <c r="D186" s="32"/>
+      <c r="E186" s="32"/>
       <c r="F186" s="16"/>
       <c r="G186" s="16"/>
       <c r="H186" s="18"/>
       <c r="I186" s="19"/>
       <c r="J186" s="16"/>
       <c r="K186" s="16"/>
-      <c r="L186" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M186" s="19" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.5" outlineLevel="0" r="187">
-      <c r="B187" s="30" t="s">
-        <v>356</v>
-      </c>
-      <c r="C187" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D187" s="32" t="s">
-        <v>351</v>
-      </c>
-      <c r="E187" s="32" t="s">
-        <v>352</v>
-      </c>
+      <c r="L186" s="18"/>
+      <c r="M186" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="187">
+      <c r="B187" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="C187" s="31"/>
+      <c r="D187" s="32"/>
+      <c r="E187" s="32"/>
       <c r="F187" s="16"/>
       <c r="G187" s="16"/>
       <c r="H187" s="18"/>
       <c r="I187" s="19"/>
       <c r="J187" s="16"/>
       <c r="K187" s="16"/>
-      <c r="L187" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M187" s="19" t="s">
-        <v>349</v>
-      </c>
+      <c r="L187" s="18"/>
+      <c r="M187" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="188">
-      <c r="B188" s="30" t="s">
-        <v>357</v>
-      </c>
-      <c r="C188" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D188" s="32" t="s">
-        <v>347</v>
-      </c>
-      <c r="E188" s="32" t="s">
-        <v>348</v>
-      </c>
+      <c r="B188" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="C188" s="31"/>
+      <c r="D188" s="32"/>
+      <c r="E188" s="32"/>
       <c r="F188" s="16"/>
       <c r="G188" s="16"/>
       <c r="H188" s="18"/>
       <c r="I188" s="19"/>
       <c r="J188" s="16"/>
       <c r="K188" s="16"/>
-      <c r="L188" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M188" s="19" t="s">
-        <v>349</v>
-      </c>
+      <c r="L188" s="18"/>
+      <c r="M188" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="189">
-      <c r="B189" s="30" t="s">
-        <v>358</v>
-      </c>
-      <c r="C189" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D189" s="32" t="s">
-        <v>347</v>
-      </c>
-      <c r="E189" s="32" t="s">
-        <v>348</v>
-      </c>
+      <c r="B189" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="C189" s="31"/>
+      <c r="D189" s="32"/>
+      <c r="E189" s="32"/>
       <c r="F189" s="16"/>
       <c r="G189" s="16"/>
       <c r="H189" s="18"/>
       <c r="I189" s="19"/>
       <c r="J189" s="16"/>
       <c r="K189" s="16"/>
-      <c r="L189" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M189" s="19" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.5" outlineLevel="0" r="190">
-      <c r="B190" s="30" t="s">
-        <v>359</v>
-      </c>
-      <c r="C190" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D190" s="32" t="s">
-        <v>351</v>
-      </c>
-      <c r="E190" s="32" t="s">
-        <v>352</v>
-      </c>
+      <c r="L189" s="18"/>
+      <c r="M189" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="190">
+      <c r="B190" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="C190" s="31"/>
+      <c r="D190" s="32"/>
+      <c r="E190" s="32"/>
       <c r="F190" s="16"/>
       <c r="G190" s="16"/>
       <c r="H190" s="18"/>
       <c r="I190" s="19"/>
       <c r="J190" s="16"/>
       <c r="K190" s="16"/>
-      <c r="L190" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M190" s="19" t="s">
-        <v>349</v>
-      </c>
+      <c r="L190" s="18"/>
+      <c r="M190" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="191">
-      <c r="B191" s="30" t="s">
-        <v>360</v>
-      </c>
-      <c r="C191" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D191" s="32" t="s">
-        <v>347</v>
-      </c>
-      <c r="E191" s="32" t="s">
-        <v>348</v>
-      </c>
+      <c r="B191" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="C191" s="31"/>
+      <c r="D191" s="32"/>
+      <c r="E191" s="32"/>
       <c r="F191" s="16"/>
       <c r="G191" s="16"/>
       <c r="H191" s="18"/>
       <c r="I191" s="19"/>
       <c r="J191" s="16"/>
       <c r="K191" s="16"/>
-      <c r="L191" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M191" s="19" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="53.25" outlineLevel="0" r="192">
-      <c r="B192" s="30" t="s">
-        <v>361</v>
-      </c>
-      <c r="C192" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D192" s="32" t="s">
-        <v>351</v>
-      </c>
-      <c r="E192" s="32" t="s">
-        <v>352</v>
-      </c>
+      <c r="L191" s="18"/>
+      <c r="M191" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="192">
+      <c r="B192" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="C192" s="31"/>
+      <c r="D192" s="32"/>
+      <c r="E192" s="32"/>
       <c r="F192" s="16"/>
       <c r="G192" s="16"/>
       <c r="H192" s="18"/>
       <c r="I192" s="19"/>
       <c r="J192" s="16"/>
       <c r="K192" s="16"/>
-      <c r="L192" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M192" s="19" t="s">
-        <v>349</v>
-      </c>
+      <c r="L192" s="18"/>
+      <c r="M192" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="193">
-      <c r="B193" s="30" t="s">
-        <v>362</v>
-      </c>
-      <c r="C193" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D193" s="32" t="s">
-        <v>363</v>
-      </c>
-      <c r="E193" s="32" t="s">
-        <v>364</v>
-      </c>
+      <c r="B193" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="C193" s="31"/>
+      <c r="D193" s="32"/>
+      <c r="E193" s="32"/>
       <c r="F193" s="16"/>
       <c r="G193" s="16"/>
       <c r="H193" s="18"/>
       <c r="I193" s="19"/>
       <c r="J193" s="16"/>
       <c r="K193" s="16"/>
-      <c r="L193" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M193" s="19" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="194">
-      <c r="A194" s="22"/>
-      <c r="B194" s="23"/>
-      <c r="C194" s="23"/>
-      <c r="D194" s="23"/>
-      <c r="E194" s="24"/>
-      <c r="F194" s="60"/>
-      <c r="G194" s="60"/>
-      <c r="H194" s="61"/>
-      <c r="I194" s="62"/>
-      <c r="J194" s="60"/>
-      <c r="K194" s="60"/>
-      <c r="L194" s="61"/>
-      <c r="M194" s="62"/>
-      <c r="N194" s="28"/>
-      <c r="O194" s="28"/>
-      <c r="P194" s="28"/>
-      <c r="Q194" s="28"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="195">
-      <c r="B195" s="15" t="s">
-        <v>365</v>
-      </c>
+      <c r="L193" s="18"/>
+      <c r="M193" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="194">
+      <c r="B194" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="C194" s="31"/>
+      <c r="D194" s="32"/>
+      <c r="E194" s="32"/>
+      <c r="F194" s="16"/>
+      <c r="G194" s="16"/>
+      <c r="H194" s="18"/>
+      <c r="I194" s="19"/>
+      <c r="J194" s="16"/>
+      <c r="K194" s="16"/>
+      <c r="L194" s="18"/>
+      <c r="M194" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="195">
+      <c r="B195" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="C195" s="31"/>
+      <c r="D195" s="32"/>
+      <c r="E195" s="32"/>
       <c r="F195" s="16"/>
       <c r="G195" s="16"/>
       <c r="H195" s="18"/>
@@ -6848,281 +7000,173 @@
       <c r="L195" s="18"/>
       <c r="M195" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="196">
-      <c r="B196" s="30" t="s">
-        <v>366</v>
-      </c>
-      <c r="C196" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D196" s="32" t="s">
-        <v>367</v>
-      </c>
-      <c r="E196" s="32" t="s">
-        <v>368</v>
-      </c>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="196">
+      <c r="B196" s="0" t="s">
+        <v>364</v>
+      </c>
+      <c r="C196" s="31"/>
+      <c r="D196" s="32"/>
+      <c r="E196" s="32"/>
       <c r="F196" s="16"/>
       <c r="G196" s="16"/>
       <c r="H196" s="18"/>
-      <c r="I196" s="19" t="s">
-        <v>369</v>
-      </c>
+      <c r="I196" s="19"/>
       <c r="J196" s="16"/>
       <c r="K196" s="16"/>
-      <c r="L196" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M196" s="19" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="197">
-      <c r="B197" s="30" t="s">
-        <v>370</v>
-      </c>
-      <c r="C197" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D197" s="32" t="s">
-        <v>371</v>
-      </c>
-      <c r="E197" s="32" t="s">
-        <v>372</v>
-      </c>
+      <c r="L196" s="18"/>
+      <c r="M196" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="197">
+      <c r="B197" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="C197" s="31"/>
+      <c r="D197" s="32"/>
+      <c r="E197" s="32"/>
       <c r="F197" s="16"/>
       <c r="G197" s="16"/>
       <c r="H197" s="18"/>
-      <c r="I197" s="19" t="s">
-        <v>369</v>
-      </c>
+      <c r="I197" s="19"/>
       <c r="J197" s="16"/>
       <c r="K197" s="16"/>
-      <c r="L197" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M197" s="19" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="198">
-      <c r="B198" s="30" t="s">
-        <v>373</v>
-      </c>
-      <c r="C198" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D198" s="32" t="s">
-        <v>374</v>
-      </c>
-      <c r="E198" s="32" t="s">
-        <v>375</v>
-      </c>
+      <c r="L197" s="18"/>
+      <c r="M197" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="198">
+      <c r="B198" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="C198" s="31"/>
+      <c r="D198" s="32"/>
+      <c r="E198" s="32"/>
       <c r="F198" s="16"/>
       <c r="G198" s="16"/>
       <c r="H198" s="18"/>
-      <c r="I198" s="19" t="s">
-        <v>369</v>
-      </c>
+      <c r="I198" s="19"/>
       <c r="J198" s="16"/>
       <c r="K198" s="16"/>
-      <c r="L198" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M198" s="19" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="199">
-      <c r="B199" s="30" t="s">
-        <v>376</v>
-      </c>
-      <c r="C199" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D199" s="32" t="s">
-        <v>377</v>
-      </c>
-      <c r="E199" s="32" t="s">
-        <v>378</v>
-      </c>
+      <c r="L198" s="18"/>
+      <c r="M198" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="199">
+      <c r="B199" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="C199" s="31"/>
+      <c r="D199" s="32"/>
+      <c r="E199" s="32"/>
       <c r="F199" s="16"/>
       <c r="G199" s="16"/>
       <c r="H199" s="18"/>
-      <c r="I199" s="19" t="s">
-        <v>369</v>
-      </c>
+      <c r="I199" s="19"/>
       <c r="J199" s="16"/>
       <c r="K199" s="16"/>
-      <c r="L199" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M199" s="19" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="200">
-      <c r="B200" s="30" t="s">
-        <v>379</v>
-      </c>
-      <c r="C200" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D200" s="32" t="s">
-        <v>380</v>
-      </c>
-      <c r="E200" s="32" t="s">
-        <v>381</v>
-      </c>
+      <c r="L199" s="18"/>
+      <c r="M199" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="200">
+      <c r="B200" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="C200" s="31"/>
+      <c r="D200" s="32"/>
+      <c r="E200" s="32"/>
       <c r="F200" s="16"/>
       <c r="G200" s="16"/>
       <c r="H200" s="18"/>
-      <c r="I200" s="19" t="s">
-        <v>369</v>
-      </c>
+      <c r="I200" s="19"/>
       <c r="J200" s="16"/>
       <c r="K200" s="16"/>
-      <c r="L200" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M200" s="19" t="s">
+      <c r="L200" s="18"/>
+      <c r="M200" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="201">
+      <c r="B201" s="0" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="201">
-      <c r="B201" s="30" t="s">
-        <v>382</v>
-      </c>
-      <c r="C201" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D201" s="32" t="s">
-        <v>383</v>
-      </c>
-      <c r="E201" s="32" t="s">
-        <v>384</v>
-      </c>
+      <c r="C201" s="31"/>
+      <c r="D201" s="32"/>
+      <c r="E201" s="32"/>
       <c r="F201" s="16"/>
       <c r="G201" s="16"/>
       <c r="H201" s="18"/>
-      <c r="I201" s="19" t="s">
-        <v>369</v>
-      </c>
+      <c r="I201" s="19"/>
       <c r="J201" s="16"/>
       <c r="K201" s="16"/>
-      <c r="L201" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M201" s="19" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="202">
-      <c r="B202" s="30" t="s">
-        <v>385</v>
-      </c>
-      <c r="C202" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D202" s="32" t="s">
-        <v>386</v>
-      </c>
-      <c r="E202" s="32" t="s">
-        <v>387</v>
-      </c>
+      <c r="L201" s="18"/>
+      <c r="M201" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="202">
+      <c r="B202" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="C202" s="31"/>
+      <c r="D202" s="32"/>
+      <c r="E202" s="32"/>
       <c r="F202" s="16"/>
       <c r="G202" s="16"/>
       <c r="H202" s="18"/>
-      <c r="I202" s="35" t="s">
-        <v>34</v>
-      </c>
+      <c r="I202" s="19"/>
       <c r="J202" s="16"/>
       <c r="K202" s="16"/>
-      <c r="L202" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M202" s="35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45" outlineLevel="0" r="203">
-      <c r="B203" s="30" t="s">
-        <v>388</v>
-      </c>
-      <c r="C203" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D203" s="32" t="s">
-        <v>389</v>
-      </c>
-      <c r="E203" s="32" t="s">
-        <v>390</v>
-      </c>
+      <c r="L202" s="18"/>
+      <c r="M202" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="203">
+      <c r="B203" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="C203" s="31"/>
+      <c r="D203" s="32"/>
+      <c r="E203" s="32"/>
       <c r="F203" s="16"/>
       <c r="G203" s="16"/>
       <c r="H203" s="18"/>
-      <c r="I203" s="19" t="s">
-        <v>391</v>
-      </c>
+      <c r="I203" s="19"/>
       <c r="J203" s="16"/>
       <c r="K203" s="16"/>
-      <c r="L203" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M203" s="19" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45.75" outlineLevel="0" r="204">
-      <c r="B204" s="30" t="s">
-        <v>392</v>
-      </c>
-      <c r="C204" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D204" s="32" t="s">
-        <v>393</v>
-      </c>
-      <c r="E204" s="32" t="s">
-        <v>394</v>
-      </c>
+      <c r="L203" s="18"/>
+      <c r="M203" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="204">
+      <c r="B204" s="0" t="s">
+        <v>372</v>
+      </c>
+      <c r="C204" s="31"/>
+      <c r="D204" s="32"/>
+      <c r="E204" s="32"/>
       <c r="F204" s="16"/>
       <c r="G204" s="16"/>
       <c r="H204" s="18"/>
-      <c r="I204" s="19" t="s">
-        <v>391</v>
-      </c>
+      <c r="I204" s="19"/>
       <c r="J204" s="16"/>
       <c r="K204" s="16"/>
-      <c r="L204" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M204" s="19" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="205">
-      <c r="A205" s="22"/>
-      <c r="B205" s="23"/>
-      <c r="C205" s="23"/>
-      <c r="D205" s="23"/>
-      <c r="E205" s="24"/>
-      <c r="F205" s="60"/>
-      <c r="G205" s="60"/>
-      <c r="H205" s="61"/>
-      <c r="I205" s="62"/>
-      <c r="J205" s="60"/>
-      <c r="K205" s="60"/>
-      <c r="L205" s="61"/>
-      <c r="M205" s="62"/>
-      <c r="N205" s="28"/>
-      <c r="O205" s="28"/>
-      <c r="P205" s="28"/>
-      <c r="Q205" s="28"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="206">
-      <c r="B206" s="15" t="s">
-        <v>395</v>
-      </c>
+      <c r="L204" s="18"/>
+      <c r="M204" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="205">
+      <c r="B205" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="C205" s="31"/>
+      <c r="D205" s="32"/>
+      <c r="E205" s="32"/>
+      <c r="F205" s="16"/>
+      <c r="G205" s="16"/>
+      <c r="H205" s="18"/>
+      <c r="I205" s="19"/>
+      <c r="J205" s="16"/>
+      <c r="K205" s="16"/>
+      <c r="L205" s="18"/>
+      <c r="M205" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="206">
+      <c r="B206" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="C206" s="31"/>
+      <c r="D206" s="32"/>
+      <c r="E206" s="32"/>
       <c r="F206" s="16"/>
       <c r="G206" s="16"/>
       <c r="H206" s="18"/>
@@ -7132,154 +7176,93 @@
       <c r="L206" s="18"/>
       <c r="M206" s="19"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="19.2" outlineLevel="0" r="207" s="43">
-      <c r="A207" s="39"/>
-      <c r="B207" s="49" t="s">
-        <v>396</v>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="207">
+      <c r="B207" s="0" t="s">
+        <v>358</v>
       </c>
       <c r="C207" s="31"/>
-      <c r="D207" s="20"/>
-      <c r="E207" s="20"/>
-      <c r="F207" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="G207" s="51" t="inlineStr">
-        <f aca="true">NOW()</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H207" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I207" s="42" t="s">
-        <v>397</v>
-      </c>
-      <c r="J207" s="40"/>
-      <c r="K207" s="40"/>
-      <c r="L207" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="M207" s="42" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24.85" outlineLevel="0" r="208" s="43">
-      <c r="A208" s="39"/>
-      <c r="B208" s="49" t="s">
-        <v>398</v>
+      <c r="D207" s="32"/>
+      <c r="E207" s="32"/>
+      <c r="F207" s="16"/>
+      <c r="G207" s="16"/>
+      <c r="H207" s="18"/>
+      <c r="I207" s="19"/>
+      <c r="J207" s="16"/>
+      <c r="K207" s="16"/>
+      <c r="L207" s="18"/>
+      <c r="M207" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="208">
+      <c r="B208" s="0" t="s">
+        <v>375</v>
       </c>
       <c r="C208" s="31"/>
-      <c r="D208" s="20"/>
-      <c r="E208" s="20"/>
-      <c r="F208" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="G208" s="51" t="inlineStr">
-        <f aca="true">NOW()</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H208" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I208" s="42"/>
-      <c r="J208" s="40"/>
-      <c r="K208" s="40"/>
-      <c r="L208" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="M208" s="42"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="36.15" outlineLevel="0" r="209" s="43">
-      <c r="A209" s="39"/>
-      <c r="B209" s="49" t="s">
-        <v>399</v>
+      <c r="D208" s="32"/>
+      <c r="E208" s="32"/>
+      <c r="F208" s="16"/>
+      <c r="G208" s="16"/>
+      <c r="H208" s="18"/>
+      <c r="I208" s="19"/>
+      <c r="J208" s="16"/>
+      <c r="K208" s="16"/>
+      <c r="L208" s="18"/>
+      <c r="M208" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="209">
+      <c r="B209" s="0" t="s">
+        <v>376</v>
       </c>
       <c r="C209" s="31"/>
-      <c r="D209" s="20"/>
-      <c r="E209" s="20"/>
-      <c r="F209" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="G209" s="51" t="inlineStr">
-        <f aca="true">NOW()</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H209" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="I209" s="42"/>
-      <c r="J209" s="40"/>
-      <c r="K209" s="40"/>
-      <c r="L209" s="52" t="s">
-        <v>33</v>
-      </c>
-      <c r="M209" s="42" t="s">
-        <v>400</v>
-      </c>
-      <c r="N209" s="43" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30.75" outlineLevel="0" r="210" s="43">
-      <c r="A210" s="39"/>
-      <c r="B210" s="49" t="s">
-        <v>401</v>
+      <c r="D209" s="32"/>
+      <c r="E209" s="32"/>
+      <c r="F209" s="16"/>
+      <c r="G209" s="16"/>
+      <c r="H209" s="18"/>
+      <c r="I209" s="19"/>
+      <c r="J209" s="16"/>
+      <c r="K209" s="16"/>
+      <c r="L209" s="18"/>
+      <c r="M209" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="210">
+      <c r="B210" s="0" t="s">
+        <v>377</v>
       </c>
       <c r="C210" s="31"/>
-      <c r="D210" s="20"/>
-      <c r="E210" s="20"/>
-      <c r="F210" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="G210" s="51" t="inlineStr">
-        <f aca="true">NOW()</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H210" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I210" s="42" t="s">
-        <v>402</v>
-      </c>
-      <c r="J210" s="40"/>
-      <c r="K210" s="40"/>
-      <c r="L210" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="M210" s="42" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="211">
-      <c r="A211" s="22"/>
-      <c r="B211" s="23"/>
-      <c r="C211" s="23"/>
-      <c r="D211" s="23"/>
-      <c r="E211" s="24"/>
-      <c r="F211" s="60"/>
-      <c r="G211" s="60"/>
-      <c r="H211" s="61"/>
-      <c r="I211" s="62"/>
-      <c r="J211" s="60"/>
-      <c r="K211" s="60"/>
-      <c r="L211" s="61"/>
-      <c r="M211" s="62"/>
-      <c r="N211" s="28"/>
-      <c r="O211" s="28"/>
-      <c r="P211" s="28"/>
-      <c r="Q211" s="28"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="212">
-      <c r="B212" s="15" t="s">
-        <v>403</v>
-      </c>
+      <c r="D210" s="32"/>
+      <c r="E210" s="32"/>
+      <c r="F210" s="16"/>
+      <c r="G210" s="16"/>
+      <c r="H210" s="18"/>
+      <c r="I210" s="19"/>
+      <c r="J210" s="16"/>
+      <c r="K210" s="16"/>
+      <c r="L210" s="18"/>
+      <c r="M210" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="211">
+      <c r="B211" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="C211" s="31"/>
+      <c r="D211" s="32"/>
+      <c r="E211" s="32"/>
+      <c r="F211" s="16"/>
+      <c r="G211" s="16"/>
+      <c r="H211" s="18"/>
+      <c r="I211" s="19"/>
+      <c r="J211" s="16"/>
+      <c r="K211" s="16"/>
+      <c r="L211" s="18"/>
+      <c r="M211" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="212">
+      <c r="B212" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="C212" s="31"/>
+      <c r="D212" s="32"/>
+      <c r="E212" s="32"/>
       <c r="F212" s="16"/>
       <c r="G212" s="16"/>
       <c r="H212" s="18"/>
@@ -7289,159 +7272,93 @@
       <c r="L212" s="18"/>
       <c r="M212" s="19"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="213" s="43">
-      <c r="A213" s="50"/>
-      <c r="B213" s="56" t="s">
-        <v>404</v>
-      </c>
-      <c r="C213" s="58" t="s">
-        <v>279</v>
-      </c>
-      <c r="D213" s="20"/>
-      <c r="E213" s="20"/>
-      <c r="F213" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="G213" s="51" t="inlineStr">
-        <f aca="true">NOW()</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H213" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I213" s="42" t="s">
-        <v>405</v>
-      </c>
-      <c r="J213" s="40"/>
-      <c r="K213" s="40"/>
-      <c r="L213" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="M213" s="42"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="214" s="43">
-      <c r="A214" s="50"/>
-      <c r="B214" s="56" t="s">
-        <v>406</v>
-      </c>
-      <c r="C214" s="58" t="s">
-        <v>279</v>
-      </c>
-      <c r="D214" s="20"/>
-      <c r="E214" s="20"/>
-      <c r="F214" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="G214" s="51" t="inlineStr">
-        <f aca="true">NOW()</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H214" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I214" s="42" t="s">
-        <v>405</v>
-      </c>
-      <c r="J214" s="40"/>
-      <c r="K214" s="40"/>
-      <c r="L214" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="M214" s="42"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="215" s="43">
-      <c r="A215" s="50"/>
-      <c r="B215" s="56" t="s">
-        <v>407</v>
-      </c>
-      <c r="C215" s="58" t="s">
-        <v>279</v>
-      </c>
-      <c r="D215" s="20"/>
-      <c r="E215" s="20"/>
-      <c r="F215" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="G215" s="51" t="inlineStr">
-        <f aca="true">NOW()</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H215" s="52" t="n">
-        <v>9</v>
-      </c>
-      <c r="I215" s="42"/>
-      <c r="J215" s="40"/>
-      <c r="K215" s="40"/>
-      <c r="L215" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="M215" s="42" t="s">
-        <v>408</v>
-      </c>
-      <c r="N215" s="43" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="44.05" outlineLevel="0" r="216" s="43">
-      <c r="A216" s="50"/>
-      <c r="B216" s="56" t="s">
-        <v>409</v>
-      </c>
-      <c r="C216" s="58" t="s">
-        <v>279</v>
-      </c>
-      <c r="D216" s="20"/>
-      <c r="E216" s="20"/>
-      <c r="F216" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="G216" s="51" t="inlineStr">
-        <f aca="true">NOW()</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H216" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="I216" s="42" t="s">
-        <v>410</v>
-      </c>
-      <c r="J216" s="40"/>
-      <c r="K216" s="40"/>
-      <c r="L216" s="52" t="s">
-        <v>33</v>
-      </c>
-      <c r="M216" s="42"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="217" s="43">
-      <c r="A217" s="50"/>
-      <c r="B217" s="56" t="s">
-        <v>411</v>
-      </c>
-      <c r="C217" s="58" t="s">
-        <v>279</v>
-      </c>
-      <c r="D217" s="20"/>
-      <c r="E217" s="20"/>
-      <c r="F217" s="40"/>
-      <c r="G217" s="40"/>
-      <c r="H217" s="52"/>
-      <c r="I217" s="42"/>
-      <c r="J217" s="40"/>
-      <c r="K217" s="40"/>
-      <c r="L217" s="52" t="s">
-        <v>33</v>
-      </c>
-      <c r="M217" s="42"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="218">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="213">
+      <c r="B213" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="C213" s="31"/>
+      <c r="D213" s="32"/>
+      <c r="E213" s="32"/>
+      <c r="F213" s="16"/>
+      <c r="G213" s="16"/>
+      <c r="H213" s="18"/>
+      <c r="I213" s="19"/>
+      <c r="J213" s="16"/>
+      <c r="K213" s="16"/>
+      <c r="L213" s="18"/>
+      <c r="M213" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="214">
+      <c r="B214" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="C214" s="31"/>
+      <c r="D214" s="32"/>
+      <c r="E214" s="32"/>
+      <c r="F214" s="16"/>
+      <c r="G214" s="16"/>
+      <c r="H214" s="18"/>
+      <c r="I214" s="19"/>
+      <c r="J214" s="16"/>
+      <c r="K214" s="16"/>
+      <c r="L214" s="18"/>
+      <c r="M214" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="215">
+      <c r="B215" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="C215" s="31"/>
+      <c r="D215" s="32"/>
+      <c r="E215" s="32"/>
+      <c r="F215" s="16"/>
+      <c r="G215" s="16"/>
+      <c r="H215" s="18"/>
+      <c r="I215" s="19"/>
+      <c r="J215" s="16"/>
+      <c r="K215" s="16"/>
+      <c r="L215" s="18"/>
+      <c r="M215" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="216">
+      <c r="B216" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="C216" s="31"/>
+      <c r="D216" s="32"/>
+      <c r="E216" s="32"/>
+      <c r="F216" s="16"/>
+      <c r="G216" s="16"/>
+      <c r="H216" s="18"/>
+      <c r="I216" s="19"/>
+      <c r="J216" s="16"/>
+      <c r="K216" s="16"/>
+      <c r="L216" s="18"/>
+      <c r="M216" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="217">
+      <c r="B217" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="C217" s="31"/>
+      <c r="D217" s="32"/>
+      <c r="E217" s="32"/>
+      <c r="F217" s="16"/>
+      <c r="G217" s="16"/>
+      <c r="H217" s="18"/>
+      <c r="I217" s="19"/>
+      <c r="J217" s="16"/>
+      <c r="K217" s="16"/>
+      <c r="L217" s="18"/>
+      <c r="M217" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="218">
+      <c r="B218" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="C218" s="31"/>
+      <c r="D218" s="32"/>
+      <c r="E218" s="32"/>
       <c r="F218" s="16"/>
       <c r="G218" s="16"/>
       <c r="H218" s="18"/>
@@ -7451,7 +7368,13 @@
       <c r="L218" s="18"/>
       <c r="M218" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="219">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="219">
+      <c r="B219" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="C219" s="31"/>
+      <c r="D219" s="32"/>
+      <c r="E219" s="32"/>
       <c r="F219" s="16"/>
       <c r="G219" s="16"/>
       <c r="H219" s="18"/>
@@ -7461,7 +7384,13 @@
       <c r="L219" s="18"/>
       <c r="M219" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="220">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="220">
+      <c r="B220" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="C220" s="31"/>
+      <c r="D220" s="32"/>
+      <c r="E220" s="32"/>
       <c r="F220" s="16"/>
       <c r="G220" s="16"/>
       <c r="H220" s="18"/>
@@ -7471,7 +7400,13 @@
       <c r="L220" s="18"/>
       <c r="M220" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="221">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="221">
+      <c r="B221" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="C221" s="31"/>
+      <c r="D221" s="32"/>
+      <c r="E221" s="32"/>
       <c r="F221" s="16"/>
       <c r="G221" s="16"/>
       <c r="H221" s="18"/>
@@ -7481,81 +7416,1956 @@
       <c r="L221" s="18"/>
       <c r="M221" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="222">
-      <c r="A222" s="22"/>
-      <c r="B222" s="23"/>
-      <c r="C222" s="23"/>
-      <c r="D222" s="23"/>
-      <c r="E222" s="23"/>
-      <c r="F222" s="63"/>
-      <c r="G222" s="63"/>
-      <c r="H222" s="26"/>
-      <c r="I222" s="27"/>
-      <c r="J222" s="63"/>
-      <c r="K222" s="63"/>
-      <c r="L222" s="26"/>
-      <c r="M222" s="27"/>
-      <c r="N222" s="28"/>
-      <c r="O222" s="28"/>
-      <c r="P222" s="28"/>
-      <c r="Q222" s="28"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="223">
-      <c r="A223" s="22"/>
-      <c r="B223" s="23"/>
-      <c r="C223" s="23"/>
-      <c r="D223" s="23"/>
-      <c r="E223" s="23"/>
-      <c r="F223" s="64"/>
-      <c r="G223" s="64"/>
-      <c r="H223" s="65"/>
-      <c r="I223" s="27"/>
-      <c r="J223" s="64"/>
-      <c r="K223" s="64"/>
-      <c r="L223" s="65"/>
-      <c r="M223" s="27"/>
-      <c r="N223" s="28"/>
-      <c r="O223" s="28"/>
-      <c r="P223" s="28"/>
-      <c r="Q223" s="28"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="224">
-      <c r="A224" s="22"/>
-      <c r="B224" s="23"/>
-      <c r="C224" s="23"/>
-      <c r="D224" s="23"/>
-      <c r="E224" s="23"/>
-      <c r="F224" s="64"/>
-      <c r="G224" s="64"/>
-      <c r="H224" s="65"/>
-      <c r="I224" s="27"/>
-      <c r="J224" s="64"/>
-      <c r="K224" s="64"/>
-      <c r="L224" s="65"/>
-      <c r="M224" s="27"/>
-      <c r="N224" s="28"/>
-      <c r="O224" s="28"/>
-      <c r="P224" s="28"/>
-      <c r="Q224" s="28"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="225">
-      <c r="A225" s="22"/>
-      <c r="B225" s="23"/>
-      <c r="C225" s="23"/>
-      <c r="D225" s="23"/>
-      <c r="E225" s="23"/>
-      <c r="F225" s="64"/>
-      <c r="G225" s="64"/>
-      <c r="H225" s="65"/>
-      <c r="I225" s="27"/>
-      <c r="J225" s="64"/>
-      <c r="K225" s="64"/>
-      <c r="L225" s="65"/>
-      <c r="M225" s="27"/>
-      <c r="N225" s="28"/>
-      <c r="O225" s="28"/>
-      <c r="P225" s="28"/>
-      <c r="Q225" s="28"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="222">
+      <c r="B222" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="C222" s="31"/>
+      <c r="D222" s="32"/>
+      <c r="E222" s="32"/>
+      <c r="F222" s="16"/>
+      <c r="G222" s="16"/>
+      <c r="H222" s="18"/>
+      <c r="I222" s="19"/>
+      <c r="J222" s="16"/>
+      <c r="K222" s="16"/>
+      <c r="L222" s="18"/>
+      <c r="M222" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="223">
+      <c r="B223" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="C223" s="31"/>
+      <c r="D223" s="32"/>
+      <c r="E223" s="32"/>
+      <c r="F223" s="16"/>
+      <c r="G223" s="16"/>
+      <c r="H223" s="18"/>
+      <c r="I223" s="19"/>
+      <c r="J223" s="16"/>
+      <c r="K223" s="16"/>
+      <c r="L223" s="18"/>
+      <c r="M223" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="224">
+      <c r="B224" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="C224" s="31"/>
+      <c r="D224" s="32"/>
+      <c r="E224" s="32"/>
+      <c r="F224" s="16"/>
+      <c r="G224" s="16"/>
+      <c r="H224" s="18"/>
+      <c r="I224" s="19"/>
+      <c r="J224" s="16"/>
+      <c r="K224" s="16"/>
+      <c r="L224" s="18"/>
+      <c r="M224" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="225">
+      <c r="B225" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="C225" s="31"/>
+      <c r="D225" s="32"/>
+      <c r="E225" s="32"/>
+      <c r="F225" s="16"/>
+      <c r="G225" s="16"/>
+      <c r="H225" s="18"/>
+      <c r="I225" s="19"/>
+      <c r="J225" s="16"/>
+      <c r="K225" s="16"/>
+      <c r="L225" s="18"/>
+      <c r="M225" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="226">
+      <c r="B226" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="C226" s="31"/>
+      <c r="D226" s="32"/>
+      <c r="E226" s="32"/>
+      <c r="F226" s="16"/>
+      <c r="G226" s="16"/>
+      <c r="H226" s="18"/>
+      <c r="I226" s="19"/>
+      <c r="J226" s="16"/>
+      <c r="K226" s="16"/>
+      <c r="L226" s="18"/>
+      <c r="M226" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="227">
+      <c r="B227" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="C227" s="31"/>
+      <c r="D227" s="32"/>
+      <c r="E227" s="32"/>
+      <c r="F227" s="16"/>
+      <c r="G227" s="16"/>
+      <c r="H227" s="18"/>
+      <c r="I227" s="19"/>
+      <c r="J227" s="16"/>
+      <c r="K227" s="16"/>
+      <c r="L227" s="18"/>
+      <c r="M227" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="228">
+      <c r="B228" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="C228" s="31"/>
+      <c r="D228" s="32"/>
+      <c r="E228" s="32"/>
+      <c r="F228" s="16"/>
+      <c r="G228" s="16"/>
+      <c r="H228" s="18"/>
+      <c r="I228" s="19"/>
+      <c r="J228" s="16"/>
+      <c r="K228" s="16"/>
+      <c r="L228" s="18"/>
+      <c r="M228" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="229">
+      <c r="B229" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="C229" s="31"/>
+      <c r="D229" s="32"/>
+      <c r="E229" s="32"/>
+      <c r="F229" s="16"/>
+      <c r="G229" s="16"/>
+      <c r="H229" s="18"/>
+      <c r="I229" s="19"/>
+      <c r="J229" s="16"/>
+      <c r="K229" s="16"/>
+      <c r="L229" s="18"/>
+      <c r="M229" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="230">
+      <c r="B230" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="C230" s="31"/>
+      <c r="D230" s="32"/>
+      <c r="E230" s="32"/>
+      <c r="F230" s="16"/>
+      <c r="G230" s="16"/>
+      <c r="H230" s="18"/>
+      <c r="I230" s="19"/>
+      <c r="J230" s="16"/>
+      <c r="K230" s="16"/>
+      <c r="L230" s="18"/>
+      <c r="M230" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="231">
+      <c r="B231" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="C231" s="31"/>
+      <c r="D231" s="32"/>
+      <c r="E231" s="32"/>
+      <c r="F231" s="16"/>
+      <c r="G231" s="16"/>
+      <c r="H231" s="18"/>
+      <c r="I231" s="19"/>
+      <c r="J231" s="16"/>
+      <c r="K231" s="16"/>
+      <c r="L231" s="18"/>
+      <c r="M231" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="232">
+      <c r="B232" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="C232" s="31"/>
+      <c r="D232" s="32"/>
+      <c r="E232" s="32"/>
+      <c r="F232" s="16"/>
+      <c r="G232" s="16"/>
+      <c r="H232" s="18"/>
+      <c r="I232" s="19"/>
+      <c r="J232" s="16"/>
+      <c r="K232" s="16"/>
+      <c r="L232" s="18"/>
+      <c r="M232" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="233">
+      <c r="B233" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="C233" s="31"/>
+      <c r="D233" s="32"/>
+      <c r="E233" s="32"/>
+      <c r="F233" s="16"/>
+      <c r="G233" s="16"/>
+      <c r="H233" s="18"/>
+      <c r="I233" s="19"/>
+      <c r="J233" s="16"/>
+      <c r="K233" s="16"/>
+      <c r="L233" s="18"/>
+      <c r="M233" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="234">
+      <c r="B234" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="C234" s="31"/>
+      <c r="D234" s="32"/>
+      <c r="E234" s="32"/>
+      <c r="F234" s="16"/>
+      <c r="G234" s="16"/>
+      <c r="H234" s="18"/>
+      <c r="I234" s="19"/>
+      <c r="J234" s="16"/>
+      <c r="K234" s="16"/>
+      <c r="L234" s="18"/>
+      <c r="M234" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="235">
+      <c r="B235" s="0" t="s">
+        <v>402</v>
+      </c>
+      <c r="C235" s="31"/>
+      <c r="D235" s="32"/>
+      <c r="E235" s="32"/>
+      <c r="F235" s="16"/>
+      <c r="G235" s="16"/>
+      <c r="H235" s="18"/>
+      <c r="I235" s="19"/>
+      <c r="J235" s="16"/>
+      <c r="K235" s="16"/>
+      <c r="L235" s="18"/>
+      <c r="M235" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="236">
+      <c r="B236" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="C236" s="31"/>
+      <c r="D236" s="32"/>
+      <c r="E236" s="32"/>
+      <c r="F236" s="16"/>
+      <c r="G236" s="16"/>
+      <c r="H236" s="18"/>
+      <c r="I236" s="19"/>
+      <c r="J236" s="16"/>
+      <c r="K236" s="16"/>
+      <c r="L236" s="18"/>
+      <c r="M236" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="237">
+      <c r="B237" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="C237" s="31"/>
+      <c r="D237" s="32"/>
+      <c r="E237" s="32"/>
+      <c r="F237" s="16"/>
+      <c r="G237" s="16"/>
+      <c r="H237" s="18"/>
+      <c r="I237" s="19"/>
+      <c r="J237" s="16"/>
+      <c r="K237" s="16"/>
+      <c r="L237" s="18"/>
+      <c r="M237" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="238">
+      <c r="B238" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="C238" s="31"/>
+      <c r="D238" s="32"/>
+      <c r="E238" s="32"/>
+      <c r="F238" s="16"/>
+      <c r="G238" s="16"/>
+      <c r="H238" s="18"/>
+      <c r="I238" s="19"/>
+      <c r="J238" s="16"/>
+      <c r="K238" s="16"/>
+      <c r="L238" s="18"/>
+      <c r="M238" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="239">
+      <c r="B239" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="C239" s="31"/>
+      <c r="D239" s="32"/>
+      <c r="E239" s="32"/>
+      <c r="F239" s="16"/>
+      <c r="G239" s="16"/>
+      <c r="H239" s="18"/>
+      <c r="I239" s="19"/>
+      <c r="J239" s="16"/>
+      <c r="K239" s="16"/>
+      <c r="L239" s="18"/>
+      <c r="M239" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="240">
+      <c r="B240" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="C240" s="31"/>
+      <c r="D240" s="32"/>
+      <c r="E240" s="32"/>
+      <c r="F240" s="16"/>
+      <c r="G240" s="16"/>
+      <c r="H240" s="18"/>
+      <c r="I240" s="19"/>
+      <c r="J240" s="16"/>
+      <c r="K240" s="16"/>
+      <c r="L240" s="18"/>
+      <c r="M240" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="241">
+      <c r="B241" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="C241" s="31"/>
+      <c r="D241" s="32"/>
+      <c r="E241" s="32"/>
+      <c r="F241" s="16"/>
+      <c r="G241" s="16"/>
+      <c r="H241" s="18"/>
+      <c r="I241" s="19"/>
+      <c r="J241" s="16"/>
+      <c r="K241" s="16"/>
+      <c r="L241" s="18"/>
+      <c r="M241" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="242">
+      <c r="B242" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="C242" s="31"/>
+      <c r="D242" s="32"/>
+      <c r="E242" s="32"/>
+      <c r="F242" s="16"/>
+      <c r="G242" s="16"/>
+      <c r="H242" s="18"/>
+      <c r="I242" s="19"/>
+      <c r="J242" s="16"/>
+      <c r="K242" s="16"/>
+      <c r="L242" s="18"/>
+      <c r="M242" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="243">
+      <c r="B243" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="C243" s="31"/>
+      <c r="D243" s="32"/>
+      <c r="E243" s="32"/>
+      <c r="F243" s="16"/>
+      <c r="G243" s="16"/>
+      <c r="H243" s="18"/>
+      <c r="I243" s="19"/>
+      <c r="J243" s="16"/>
+      <c r="K243" s="16"/>
+      <c r="L243" s="18"/>
+      <c r="M243" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="244">
+      <c r="B244" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="C244" s="31"/>
+      <c r="D244" s="32"/>
+      <c r="E244" s="32"/>
+      <c r="F244" s="16"/>
+      <c r="G244" s="16"/>
+      <c r="H244" s="18"/>
+      <c r="I244" s="19"/>
+      <c r="J244" s="16"/>
+      <c r="K244" s="16"/>
+      <c r="L244" s="18"/>
+      <c r="M244" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="245">
+      <c r="B245" s="0" t="s">
+        <v>412</v>
+      </c>
+      <c r="C245" s="31"/>
+      <c r="D245" s="32"/>
+      <c r="E245" s="32"/>
+      <c r="F245" s="16"/>
+      <c r="G245" s="16"/>
+      <c r="H245" s="18"/>
+      <c r="I245" s="19"/>
+      <c r="J245" s="16"/>
+      <c r="K245" s="16"/>
+      <c r="L245" s="18"/>
+      <c r="M245" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="246">
+      <c r="B246" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="C246" s="31"/>
+      <c r="D246" s="32"/>
+      <c r="E246" s="32"/>
+      <c r="F246" s="16"/>
+      <c r="G246" s="16"/>
+      <c r="H246" s="18"/>
+      <c r="I246" s="19"/>
+      <c r="J246" s="16"/>
+      <c r="K246" s="16"/>
+      <c r="L246" s="18"/>
+      <c r="M246" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="247">
+      <c r="B247" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="C247" s="31"/>
+      <c r="D247" s="32"/>
+      <c r="E247" s="32"/>
+      <c r="F247" s="16"/>
+      <c r="G247" s="16"/>
+      <c r="H247" s="18"/>
+      <c r="I247" s="19"/>
+      <c r="J247" s="16"/>
+      <c r="K247" s="16"/>
+      <c r="L247" s="18"/>
+      <c r="M247" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="248">
+      <c r="B248" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="C248" s="31"/>
+      <c r="D248" s="32"/>
+      <c r="E248" s="32"/>
+      <c r="F248" s="16"/>
+      <c r="G248" s="16"/>
+      <c r="H248" s="18"/>
+      <c r="I248" s="19"/>
+      <c r="J248" s="16"/>
+      <c r="K248" s="16"/>
+      <c r="L248" s="18"/>
+      <c r="M248" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="249">
+      <c r="B249" s="0" t="s">
+        <v>416</v>
+      </c>
+      <c r="C249" s="31"/>
+      <c r="D249" s="32"/>
+      <c r="E249" s="32"/>
+      <c r="F249" s="16"/>
+      <c r="G249" s="16"/>
+      <c r="H249" s="18"/>
+      <c r="I249" s="19"/>
+      <c r="J249" s="16"/>
+      <c r="K249" s="16"/>
+      <c r="L249" s="18"/>
+      <c r="M249" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="250">
+      <c r="B250" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="C250" s="31"/>
+      <c r="D250" s="32"/>
+      <c r="E250" s="32"/>
+      <c r="F250" s="16"/>
+      <c r="G250" s="16"/>
+      <c r="H250" s="18"/>
+      <c r="I250" s="19"/>
+      <c r="J250" s="16"/>
+      <c r="K250" s="16"/>
+      <c r="L250" s="18"/>
+      <c r="M250" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="251">
+      <c r="B251" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="C251" s="31"/>
+      <c r="D251" s="32"/>
+      <c r="E251" s="32"/>
+      <c r="F251" s="16"/>
+      <c r="G251" s="16"/>
+      <c r="H251" s="18"/>
+      <c r="I251" s="19"/>
+      <c r="J251" s="16"/>
+      <c r="K251" s="16"/>
+      <c r="L251" s="18"/>
+      <c r="M251" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="252">
+      <c r="B252" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="C252" s="31"/>
+      <c r="D252" s="32"/>
+      <c r="E252" s="32"/>
+      <c r="F252" s="16"/>
+      <c r="G252" s="16"/>
+      <c r="H252" s="18"/>
+      <c r="I252" s="19"/>
+      <c r="J252" s="16"/>
+      <c r="K252" s="16"/>
+      <c r="L252" s="18"/>
+      <c r="M252" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="253">
+      <c r="B253" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="C253" s="31"/>
+      <c r="D253" s="32"/>
+      <c r="E253" s="32"/>
+      <c r="F253" s="16"/>
+      <c r="G253" s="16"/>
+      <c r="H253" s="18"/>
+      <c r="I253" s="19"/>
+      <c r="J253" s="16"/>
+      <c r="K253" s="16"/>
+      <c r="L253" s="18"/>
+      <c r="M253" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="254">
+      <c r="B254" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="C254" s="31"/>
+      <c r="D254" s="32"/>
+      <c r="E254" s="32"/>
+      <c r="F254" s="16"/>
+      <c r="G254" s="16"/>
+      <c r="H254" s="18"/>
+      <c r="I254" s="19"/>
+      <c r="J254" s="16"/>
+      <c r="K254" s="16"/>
+      <c r="L254" s="18"/>
+      <c r="M254" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="255">
+      <c r="B255" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="C255" s="31"/>
+      <c r="D255" s="32"/>
+      <c r="E255" s="32"/>
+      <c r="F255" s="16"/>
+      <c r="G255" s="16"/>
+      <c r="H255" s="18"/>
+      <c r="I255" s="19"/>
+      <c r="J255" s="16"/>
+      <c r="K255" s="16"/>
+      <c r="L255" s="18"/>
+      <c r="M255" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="256">
+      <c r="B256" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="C256" s="31"/>
+      <c r="D256" s="32"/>
+      <c r="E256" s="32"/>
+      <c r="F256" s="16"/>
+      <c r="G256" s="16"/>
+      <c r="H256" s="18"/>
+      <c r="I256" s="19"/>
+      <c r="J256" s="16"/>
+      <c r="K256" s="16"/>
+      <c r="L256" s="18"/>
+      <c r="M256" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="257">
+      <c r="B257" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="C257" s="31"/>
+      <c r="D257" s="32"/>
+      <c r="E257" s="32"/>
+      <c r="F257" s="16"/>
+      <c r="G257" s="16"/>
+      <c r="H257" s="18"/>
+      <c r="I257" s="19"/>
+      <c r="J257" s="16"/>
+      <c r="K257" s="16"/>
+      <c r="L257" s="18"/>
+      <c r="M257" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="258">
+      <c r="B258" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="C258" s="31"/>
+      <c r="D258" s="32"/>
+      <c r="E258" s="32"/>
+      <c r="F258" s="16"/>
+      <c r="G258" s="16"/>
+      <c r="H258" s="18"/>
+      <c r="I258" s="19"/>
+      <c r="J258" s="16"/>
+      <c r="K258" s="16"/>
+      <c r="L258" s="18"/>
+      <c r="M258" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="259">
+      <c r="B259" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="C259" s="31"/>
+      <c r="D259" s="32"/>
+      <c r="E259" s="32"/>
+      <c r="F259" s="16"/>
+      <c r="G259" s="16"/>
+      <c r="H259" s="18"/>
+      <c r="I259" s="19"/>
+      <c r="J259" s="16"/>
+      <c r="K259" s="16"/>
+      <c r="L259" s="18"/>
+      <c r="M259" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="260">
+      <c r="B260" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="C260" s="31"/>
+      <c r="D260" s="32"/>
+      <c r="E260" s="32"/>
+      <c r="F260" s="16"/>
+      <c r="G260" s="16"/>
+      <c r="H260" s="18"/>
+      <c r="I260" s="19"/>
+      <c r="J260" s="16"/>
+      <c r="K260" s="16"/>
+      <c r="L260" s="18"/>
+      <c r="M260" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="261">
+      <c r="B261" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="C261" s="31"/>
+      <c r="D261" s="32"/>
+      <c r="E261" s="32"/>
+      <c r="F261" s="16"/>
+      <c r="G261" s="16"/>
+      <c r="H261" s="18"/>
+      <c r="I261" s="19"/>
+      <c r="J261" s="16"/>
+      <c r="K261" s="16"/>
+      <c r="L261" s="18"/>
+      <c r="M261" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="262">
+      <c r="B262" s="0" t="s">
+        <v>428</v>
+      </c>
+      <c r="C262" s="31"/>
+      <c r="D262" s="32"/>
+      <c r="E262" s="32"/>
+      <c r="F262" s="16"/>
+      <c r="G262" s="16"/>
+      <c r="H262" s="18"/>
+      <c r="I262" s="19"/>
+      <c r="J262" s="16"/>
+      <c r="K262" s="16"/>
+      <c r="L262" s="18"/>
+      <c r="M262" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="263">
+      <c r="B263" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="C263" s="31"/>
+      <c r="D263" s="32"/>
+      <c r="E263" s="32"/>
+      <c r="F263" s="16"/>
+      <c r="G263" s="16"/>
+      <c r="H263" s="18"/>
+      <c r="I263" s="19"/>
+      <c r="J263" s="16"/>
+      <c r="K263" s="16"/>
+      <c r="L263" s="18"/>
+      <c r="M263" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="264">
+      <c r="B264" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="C264" s="31"/>
+      <c r="D264" s="32"/>
+      <c r="E264" s="32"/>
+      <c r="F264" s="16"/>
+      <c r="G264" s="16"/>
+      <c r="H264" s="18"/>
+      <c r="I264" s="19"/>
+      <c r="J264" s="16"/>
+      <c r="K264" s="16"/>
+      <c r="L264" s="18"/>
+      <c r="M264" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="265">
+      <c r="B265" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="C265" s="31"/>
+      <c r="D265" s="32"/>
+      <c r="E265" s="32"/>
+      <c r="F265" s="16"/>
+      <c r="G265" s="16"/>
+      <c r="H265" s="18"/>
+      <c r="I265" s="19"/>
+      <c r="J265" s="16"/>
+      <c r="K265" s="16"/>
+      <c r="L265" s="18"/>
+      <c r="M265" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="266">
+      <c r="B266" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="C266" s="31"/>
+      <c r="D266" s="32"/>
+      <c r="E266" s="32"/>
+      <c r="F266" s="16"/>
+      <c r="G266" s="16"/>
+      <c r="H266" s="18"/>
+      <c r="I266" s="19"/>
+      <c r="J266" s="16"/>
+      <c r="K266" s="16"/>
+      <c r="L266" s="18"/>
+      <c r="M266" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="267">
+      <c r="B267" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="C267" s="31"/>
+      <c r="D267" s="32"/>
+      <c r="E267" s="32"/>
+      <c r="F267" s="16"/>
+      <c r="G267" s="16"/>
+      <c r="H267" s="18"/>
+      <c r="I267" s="19"/>
+      <c r="J267" s="16"/>
+      <c r="K267" s="16"/>
+      <c r="L267" s="18"/>
+      <c r="M267" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="268">
+      <c r="B268" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="C268" s="31"/>
+      <c r="D268" s="32"/>
+      <c r="E268" s="32"/>
+      <c r="F268" s="16"/>
+      <c r="G268" s="16"/>
+      <c r="H268" s="18"/>
+      <c r="I268" s="19"/>
+      <c r="J268" s="16"/>
+      <c r="K268" s="16"/>
+      <c r="L268" s="18"/>
+      <c r="M268" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="269">
+      <c r="B269" s="0"/>
+      <c r="C269" s="31"/>
+      <c r="D269" s="32"/>
+      <c r="E269" s="32"/>
+      <c r="F269" s="16"/>
+      <c r="G269" s="16"/>
+      <c r="H269" s="18"/>
+      <c r="I269" s="19"/>
+      <c r="J269" s="16"/>
+      <c r="K269" s="16"/>
+      <c r="L269" s="18"/>
+      <c r="M269" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="270">
+      <c r="B270" s="0"/>
+      <c r="C270" s="31"/>
+      <c r="D270" s="32"/>
+      <c r="E270" s="32"/>
+      <c r="F270" s="16"/>
+      <c r="G270" s="16"/>
+      <c r="H270" s="18"/>
+      <c r="I270" s="19"/>
+      <c r="J270" s="16"/>
+      <c r="K270" s="16"/>
+      <c r="L270" s="18"/>
+      <c r="M270" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="271">
+      <c r="B271" s="0"/>
+      <c r="C271" s="31"/>
+      <c r="D271" s="32"/>
+      <c r="E271" s="32"/>
+      <c r="F271" s="16"/>
+      <c r="G271" s="16"/>
+      <c r="H271" s="18"/>
+      <c r="I271" s="19"/>
+      <c r="J271" s="16"/>
+      <c r="K271" s="16"/>
+      <c r="L271" s="18"/>
+      <c r="M271" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="272">
+      <c r="B272" s="0"/>
+      <c r="C272" s="31"/>
+      <c r="D272" s="32"/>
+      <c r="E272" s="32"/>
+      <c r="F272" s="16"/>
+      <c r="G272" s="16"/>
+      <c r="H272" s="18"/>
+      <c r="I272" s="19"/>
+      <c r="J272" s="16"/>
+      <c r="K272" s="16"/>
+      <c r="L272" s="18"/>
+      <c r="M272" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="273">
+      <c r="B273" s="30"/>
+      <c r="C273" s="31"/>
+      <c r="D273" s="32"/>
+      <c r="E273" s="32"/>
+      <c r="F273" s="16"/>
+      <c r="G273" s="16"/>
+      <c r="H273" s="18"/>
+      <c r="I273" s="19"/>
+      <c r="J273" s="16"/>
+      <c r="K273" s="16"/>
+      <c r="L273" s="18"/>
+      <c r="M273" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="274">
+      <c r="B274" s="30"/>
+      <c r="C274" s="31"/>
+      <c r="D274" s="32"/>
+      <c r="E274" s="32"/>
+      <c r="F274" s="16"/>
+      <c r="G274" s="16"/>
+      <c r="H274" s="18"/>
+      <c r="I274" s="19"/>
+      <c r="J274" s="16"/>
+      <c r="K274" s="16"/>
+      <c r="L274" s="18"/>
+      <c r="M274" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="275">
+      <c r="B275" s="30"/>
+      <c r="C275" s="31"/>
+      <c r="D275" s="32"/>
+      <c r="E275" s="32"/>
+      <c r="F275" s="16"/>
+      <c r="G275" s="16"/>
+      <c r="H275" s="18"/>
+      <c r="I275" s="19"/>
+      <c r="J275" s="16"/>
+      <c r="K275" s="16"/>
+      <c r="L275" s="18"/>
+      <c r="M275" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="276">
+      <c r="B276" s="30"/>
+      <c r="C276" s="31"/>
+      <c r="D276" s="32"/>
+      <c r="E276" s="32"/>
+      <c r="F276" s="16"/>
+      <c r="G276" s="16"/>
+      <c r="H276" s="18"/>
+      <c r="I276" s="19"/>
+      <c r="J276" s="16"/>
+      <c r="K276" s="16"/>
+      <c r="L276" s="18"/>
+      <c r="M276" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="277">
+      <c r="B277" s="30"/>
+      <c r="C277" s="31"/>
+      <c r="D277" s="32"/>
+      <c r="E277" s="32"/>
+      <c r="F277" s="16"/>
+      <c r="G277" s="16"/>
+      <c r="H277" s="18"/>
+      <c r="I277" s="19"/>
+      <c r="J277" s="16"/>
+      <c r="K277" s="16"/>
+      <c r="L277" s="18"/>
+      <c r="M277" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="278">
+      <c r="B278" s="30"/>
+      <c r="C278" s="31"/>
+      <c r="D278" s="32"/>
+      <c r="E278" s="32"/>
+      <c r="F278" s="16"/>
+      <c r="G278" s="16"/>
+      <c r="H278" s="18"/>
+      <c r="I278" s="19"/>
+      <c r="J278" s="16"/>
+      <c r="K278" s="16"/>
+      <c r="L278" s="18"/>
+      <c r="M278" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="279" s="65">
+      <c r="A279" s="63"/>
+      <c r="B279" s="30"/>
+      <c r="C279" s="31"/>
+      <c r="D279" s="32"/>
+      <c r="E279" s="32"/>
+      <c r="F279" s="16"/>
+      <c r="G279" s="16"/>
+      <c r="H279" s="18"/>
+      <c r="I279" s="19"/>
+      <c r="J279" s="16"/>
+      <c r="K279" s="16"/>
+      <c r="L279" s="18"/>
+      <c r="M279" s="19"/>
+      <c r="N279" s="64"/>
+      <c r="O279" s="64"/>
+      <c r="P279" s="64"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="280">
+      <c r="B280" s="30"/>
+      <c r="C280" s="31"/>
+      <c r="D280" s="32"/>
+      <c r="E280" s="32"/>
+      <c r="F280" s="16"/>
+      <c r="G280" s="16"/>
+      <c r="H280" s="18"/>
+      <c r="I280" s="19"/>
+      <c r="J280" s="16"/>
+      <c r="K280" s="16"/>
+      <c r="L280" s="18"/>
+      <c r="M280" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.5" outlineLevel="0" r="281">
+      <c r="B281" s="30" t="s">
+        <v>435</v>
+      </c>
+      <c r="C281" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D281" s="32" t="s">
+        <v>436</v>
+      </c>
+      <c r="E281" s="32" t="s">
+        <v>437</v>
+      </c>
+      <c r="F281" s="16"/>
+      <c r="G281" s="16"/>
+      <c r="H281" s="18"/>
+      <c r="I281" s="19"/>
+      <c r="J281" s="16"/>
+      <c r="K281" s="16"/>
+      <c r="L281" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M281" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="282">
+      <c r="B282" s="30" t="s">
+        <v>438</v>
+      </c>
+      <c r="C282" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D282" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="E282" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="F282" s="16"/>
+      <c r="G282" s="16"/>
+      <c r="H282" s="18"/>
+      <c r="I282" s="19"/>
+      <c r="J282" s="16"/>
+      <c r="K282" s="16"/>
+      <c r="L282" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M282" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.5" outlineLevel="0" r="283">
+      <c r="B283" s="30" t="s">
+        <v>439</v>
+      </c>
+      <c r="C283" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D283" s="32" t="s">
+        <v>436</v>
+      </c>
+      <c r="E283" s="32" t="s">
+        <v>437</v>
+      </c>
+      <c r="F283" s="16"/>
+      <c r="G283" s="16"/>
+      <c r="H283" s="18"/>
+      <c r="I283" s="19"/>
+      <c r="J283" s="16"/>
+      <c r="K283" s="16"/>
+      <c r="L283" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M283" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="284">
+      <c r="B284" s="30" t="s">
+        <v>440</v>
+      </c>
+      <c r="C284" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D284" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="E284" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="F284" s="16"/>
+      <c r="G284" s="16"/>
+      <c r="H284" s="18"/>
+      <c r="I284" s="19"/>
+      <c r="J284" s="16"/>
+      <c r="K284" s="16"/>
+      <c r="L284" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M284" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.5" outlineLevel="0" r="285">
+      <c r="B285" s="30" t="s">
+        <v>441</v>
+      </c>
+      <c r="C285" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D285" s="32" t="s">
+        <v>436</v>
+      </c>
+      <c r="E285" s="32" t="s">
+        <v>437</v>
+      </c>
+      <c r="F285" s="16"/>
+      <c r="G285" s="16"/>
+      <c r="H285" s="18"/>
+      <c r="I285" s="19"/>
+      <c r="J285" s="16"/>
+      <c r="K285" s="16"/>
+      <c r="L285" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M285" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="286">
+      <c r="B286" s="30" t="s">
+        <v>442</v>
+      </c>
+      <c r="C286" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D286" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="E286" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="F286" s="16"/>
+      <c r="G286" s="16"/>
+      <c r="H286" s="18"/>
+      <c r="I286" s="19"/>
+      <c r="J286" s="16"/>
+      <c r="K286" s="16"/>
+      <c r="L286" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M286" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="287">
+      <c r="B287" s="30" t="s">
+        <v>443</v>
+      </c>
+      <c r="C287" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D287" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="E287" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="F287" s="16"/>
+      <c r="G287" s="16"/>
+      <c r="H287" s="18"/>
+      <c r="I287" s="19"/>
+      <c r="J287" s="16"/>
+      <c r="K287" s="16"/>
+      <c r="L287" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M287" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.5" outlineLevel="0" r="288">
+      <c r="B288" s="30" t="s">
+        <v>444</v>
+      </c>
+      <c r="C288" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D288" s="32" t="s">
+        <v>436</v>
+      </c>
+      <c r="E288" s="32" t="s">
+        <v>437</v>
+      </c>
+      <c r="F288" s="16"/>
+      <c r="G288" s="16"/>
+      <c r="H288" s="18"/>
+      <c r="I288" s="19"/>
+      <c r="J288" s="16"/>
+      <c r="K288" s="16"/>
+      <c r="L288" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M288" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="289">
+      <c r="B289" s="30" t="s">
+        <v>445</v>
+      </c>
+      <c r="C289" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D289" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="E289" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="F289" s="16"/>
+      <c r="G289" s="16"/>
+      <c r="H289" s="18"/>
+      <c r="I289" s="19"/>
+      <c r="J289" s="16"/>
+      <c r="K289" s="16"/>
+      <c r="L289" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M289" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="53.25" outlineLevel="0" r="290">
+      <c r="B290" s="30" t="s">
+        <v>446</v>
+      </c>
+      <c r="C290" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D290" s="32" t="s">
+        <v>436</v>
+      </c>
+      <c r="E290" s="32" t="s">
+        <v>437</v>
+      </c>
+      <c r="F290" s="16"/>
+      <c r="G290" s="16"/>
+      <c r="H290" s="18"/>
+      <c r="I290" s="19"/>
+      <c r="J290" s="16"/>
+      <c r="K290" s="16"/>
+      <c r="L290" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M290" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="291">
+      <c r="B291" s="30" t="s">
+        <v>447</v>
+      </c>
+      <c r="C291" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D291" s="32" t="s">
+        <v>448</v>
+      </c>
+      <c r="E291" s="32" t="s">
+        <v>449</v>
+      </c>
+      <c r="F291" s="16"/>
+      <c r="G291" s="16"/>
+      <c r="H291" s="18"/>
+      <c r="I291" s="19"/>
+      <c r="J291" s="16"/>
+      <c r="K291" s="16"/>
+      <c r="L291" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M291" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="292">
+      <c r="A292" s="22"/>
+      <c r="B292" s="23"/>
+      <c r="C292" s="23"/>
+      <c r="D292" s="23"/>
+      <c r="E292" s="24"/>
+      <c r="F292" s="60"/>
+      <c r="G292" s="60"/>
+      <c r="H292" s="61"/>
+      <c r="I292" s="62"/>
+      <c r="J292" s="60"/>
+      <c r="K292" s="60"/>
+      <c r="L292" s="61"/>
+      <c r="M292" s="62"/>
+      <c r="N292" s="28"/>
+      <c r="O292" s="28"/>
+      <c r="P292" s="28"/>
+      <c r="Q292" s="28"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="293">
+      <c r="B293" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="F293" s="16"/>
+      <c r="G293" s="16"/>
+      <c r="H293" s="18"/>
+      <c r="I293" s="19"/>
+      <c r="J293" s="16"/>
+      <c r="K293" s="16"/>
+      <c r="L293" s="18"/>
+      <c r="M293" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="294">
+      <c r="B294" s="30" t="s">
+        <v>451</v>
+      </c>
+      <c r="C294" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D294" s="32" t="s">
+        <v>452</v>
+      </c>
+      <c r="E294" s="32" t="s">
+        <v>453</v>
+      </c>
+      <c r="F294" s="16"/>
+      <c r="G294" s="16"/>
+      <c r="H294" s="18"/>
+      <c r="I294" s="19" t="s">
+        <v>454</v>
+      </c>
+      <c r="J294" s="16"/>
+      <c r="K294" s="16"/>
+      <c r="L294" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M294" s="19" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="295">
+      <c r="B295" s="30" t="s">
+        <v>455</v>
+      </c>
+      <c r="C295" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D295" s="32" t="s">
+        <v>456</v>
+      </c>
+      <c r="E295" s="32" t="s">
+        <v>457</v>
+      </c>
+      <c r="F295" s="16"/>
+      <c r="G295" s="16"/>
+      <c r="H295" s="18"/>
+      <c r="I295" s="19" t="s">
+        <v>454</v>
+      </c>
+      <c r="J295" s="16"/>
+      <c r="K295" s="16"/>
+      <c r="L295" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M295" s="19" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="296">
+      <c r="B296" s="30" t="s">
+        <v>458</v>
+      </c>
+      <c r="C296" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D296" s="32" t="s">
+        <v>459</v>
+      </c>
+      <c r="E296" s="32" t="s">
+        <v>460</v>
+      </c>
+      <c r="F296" s="16"/>
+      <c r="G296" s="16"/>
+      <c r="H296" s="18"/>
+      <c r="I296" s="19" t="s">
+        <v>454</v>
+      </c>
+      <c r="J296" s="16"/>
+      <c r="K296" s="16"/>
+      <c r="L296" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M296" s="19" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="297">
+      <c r="B297" s="30" t="s">
+        <v>461</v>
+      </c>
+      <c r="C297" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D297" s="32" t="s">
+        <v>462</v>
+      </c>
+      <c r="E297" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="F297" s="16"/>
+      <c r="G297" s="16"/>
+      <c r="H297" s="18"/>
+      <c r="I297" s="19" t="s">
+        <v>454</v>
+      </c>
+      <c r="J297" s="16"/>
+      <c r="K297" s="16"/>
+      <c r="L297" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M297" s="19" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="298">
+      <c r="B298" s="30" t="s">
+        <v>464</v>
+      </c>
+      <c r="C298" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D298" s="32" t="s">
+        <v>465</v>
+      </c>
+      <c r="E298" s="32" t="s">
+        <v>466</v>
+      </c>
+      <c r="F298" s="16"/>
+      <c r="G298" s="16"/>
+      <c r="H298" s="18"/>
+      <c r="I298" s="19" t="s">
+        <v>454</v>
+      </c>
+      <c r="J298" s="16"/>
+      <c r="K298" s="16"/>
+      <c r="L298" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M298" s="19" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="299">
+      <c r="B299" s="30" t="s">
+        <v>467</v>
+      </c>
+      <c r="C299" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D299" s="32" t="s">
+        <v>468</v>
+      </c>
+      <c r="E299" s="32" t="s">
+        <v>469</v>
+      </c>
+      <c r="F299" s="16"/>
+      <c r="G299" s="16"/>
+      <c r="H299" s="18"/>
+      <c r="I299" s="19" t="s">
+        <v>454</v>
+      </c>
+      <c r="J299" s="16"/>
+      <c r="K299" s="16"/>
+      <c r="L299" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M299" s="19" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="300">
+      <c r="B300" s="30" t="s">
+        <v>470</v>
+      </c>
+      <c r="C300" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D300" s="32" t="s">
+        <v>471</v>
+      </c>
+      <c r="E300" s="32" t="s">
+        <v>472</v>
+      </c>
+      <c r="F300" s="16"/>
+      <c r="G300" s="16"/>
+      <c r="H300" s="18"/>
+      <c r="I300" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="J300" s="16"/>
+      <c r="K300" s="16"/>
+      <c r="L300" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M300" s="35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45" outlineLevel="0" r="301">
+      <c r="B301" s="30" t="s">
+        <v>473</v>
+      </c>
+      <c r="C301" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D301" s="32" t="s">
+        <v>474</v>
+      </c>
+      <c r="E301" s="32" t="s">
+        <v>475</v>
+      </c>
+      <c r="F301" s="16"/>
+      <c r="G301" s="16"/>
+      <c r="H301" s="18"/>
+      <c r="I301" s="19" t="s">
+        <v>476</v>
+      </c>
+      <c r="J301" s="16"/>
+      <c r="K301" s="16"/>
+      <c r="L301" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M301" s="19" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45.75" outlineLevel="0" r="302">
+      <c r="B302" s="30" t="s">
+        <v>477</v>
+      </c>
+      <c r="C302" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D302" s="32" t="s">
+        <v>478</v>
+      </c>
+      <c r="E302" s="32" t="s">
+        <v>479</v>
+      </c>
+      <c r="F302" s="16"/>
+      <c r="G302" s="16"/>
+      <c r="H302" s="18"/>
+      <c r="I302" s="19" t="s">
+        <v>476</v>
+      </c>
+      <c r="J302" s="16"/>
+      <c r="K302" s="16"/>
+      <c r="L302" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M302" s="19" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="303">
+      <c r="A303" s="22"/>
+      <c r="B303" s="23"/>
+      <c r="C303" s="23"/>
+      <c r="D303" s="23"/>
+      <c r="E303" s="24"/>
+      <c r="F303" s="60"/>
+      <c r="G303" s="60"/>
+      <c r="H303" s="61"/>
+      <c r="I303" s="62"/>
+      <c r="J303" s="60"/>
+      <c r="K303" s="60"/>
+      <c r="L303" s="61"/>
+      <c r="M303" s="62"/>
+      <c r="N303" s="28"/>
+      <c r="O303" s="28"/>
+      <c r="P303" s="28"/>
+      <c r="Q303" s="28"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="304">
+      <c r="B304" s="15" t="s">
+        <v>480</v>
+      </c>
+      <c r="F304" s="16"/>
+      <c r="G304" s="16"/>
+      <c r="H304" s="18"/>
+      <c r="I304" s="19"/>
+      <c r="J304" s="16"/>
+      <c r="K304" s="16"/>
+      <c r="L304" s="18"/>
+      <c r="M304" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="19.2" outlineLevel="0" r="305" s="43">
+      <c r="A305" s="39"/>
+      <c r="B305" s="49" t="s">
+        <v>481</v>
+      </c>
+      <c r="C305" s="31"/>
+      <c r="D305" s="20"/>
+      <c r="E305" s="20"/>
+      <c r="F305" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G305" s="51" t="inlineStr">
+        <f aca="true">NOW()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H305" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="I305" s="42" t="s">
+        <v>482</v>
+      </c>
+      <c r="J305" s="40"/>
+      <c r="K305" s="40"/>
+      <c r="L305" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="M305" s="42" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24.85" outlineLevel="0" r="306" s="43">
+      <c r="A306" s="39"/>
+      <c r="B306" s="49" t="s">
+        <v>483</v>
+      </c>
+      <c r="C306" s="31"/>
+      <c r="D306" s="20"/>
+      <c r="E306" s="20"/>
+      <c r="F306" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G306" s="51" t="inlineStr">
+        <f aca="true">NOW()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H306" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="I306" s="42"/>
+      <c r="J306" s="40"/>
+      <c r="K306" s="40"/>
+      <c r="L306" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="M306" s="42"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="36.15" outlineLevel="0" r="307" s="43">
+      <c r="A307" s="39"/>
+      <c r="B307" s="49" t="s">
+        <v>484</v>
+      </c>
+      <c r="C307" s="31"/>
+      <c r="D307" s="20"/>
+      <c r="E307" s="20"/>
+      <c r="F307" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G307" s="51" t="inlineStr">
+        <f aca="true">NOW()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H307" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I307" s="42"/>
+      <c r="J307" s="40"/>
+      <c r="K307" s="40"/>
+      <c r="L307" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="M307" s="42" t="s">
+        <v>485</v>
+      </c>
+      <c r="N307" s="43" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30.75" outlineLevel="0" r="308" s="43">
+      <c r="A308" s="39"/>
+      <c r="B308" s="49" t="s">
+        <v>486</v>
+      </c>
+      <c r="C308" s="31"/>
+      <c r="D308" s="20"/>
+      <c r="E308" s="20"/>
+      <c r="F308" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G308" s="51" t="inlineStr">
+        <f aca="true">NOW()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H308" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="I308" s="42" t="s">
+        <v>487</v>
+      </c>
+      <c r="J308" s="40"/>
+      <c r="K308" s="40"/>
+      <c r="L308" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="M308" s="42" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="309">
+      <c r="A309" s="22"/>
+      <c r="B309" s="23"/>
+      <c r="C309" s="23"/>
+      <c r="D309" s="23"/>
+      <c r="E309" s="24"/>
+      <c r="F309" s="60"/>
+      <c r="G309" s="60"/>
+      <c r="H309" s="61"/>
+      <c r="I309" s="62"/>
+      <c r="J309" s="60"/>
+      <c r="K309" s="60"/>
+      <c r="L309" s="61"/>
+      <c r="M309" s="62"/>
+      <c r="N309" s="28"/>
+      <c r="O309" s="28"/>
+      <c r="P309" s="28"/>
+      <c r="Q309" s="28"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="310">
+      <c r="B310" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="F310" s="16"/>
+      <c r="G310" s="16"/>
+      <c r="H310" s="18"/>
+      <c r="I310" s="19"/>
+      <c r="J310" s="16"/>
+      <c r="K310" s="16"/>
+      <c r="L310" s="18"/>
+      <c r="M310" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="311" s="43">
+      <c r="A311" s="50"/>
+      <c r="B311" s="56" t="s">
+        <v>489</v>
+      </c>
+      <c r="C311" s="58" t="s">
+        <v>279</v>
+      </c>
+      <c r="D311" s="20"/>
+      <c r="E311" s="20"/>
+      <c r="F311" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G311" s="51" t="inlineStr">
+        <f aca="true">NOW()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H311" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="I311" s="42" t="s">
+        <v>490</v>
+      </c>
+      <c r="J311" s="40"/>
+      <c r="K311" s="40"/>
+      <c r="L311" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="M311" s="42"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="312" s="43">
+      <c r="A312" s="50"/>
+      <c r="B312" s="56" t="s">
+        <v>491</v>
+      </c>
+      <c r="C312" s="58" t="s">
+        <v>279</v>
+      </c>
+      <c r="D312" s="20"/>
+      <c r="E312" s="20"/>
+      <c r="F312" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G312" s="51" t="inlineStr">
+        <f aca="true">NOW()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H312" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="I312" s="42" t="s">
+        <v>490</v>
+      </c>
+      <c r="J312" s="40"/>
+      <c r="K312" s="40"/>
+      <c r="L312" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="M312" s="42"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="313" s="43">
+      <c r="A313" s="50"/>
+      <c r="B313" s="56" t="s">
+        <v>492</v>
+      </c>
+      <c r="C313" s="58" t="s">
+        <v>279</v>
+      </c>
+      <c r="D313" s="20"/>
+      <c r="E313" s="20"/>
+      <c r="F313" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G313" s="51" t="inlineStr">
+        <f aca="true">NOW()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H313" s="52" t="n">
+        <v>9</v>
+      </c>
+      <c r="I313" s="42"/>
+      <c r="J313" s="40"/>
+      <c r="K313" s="40"/>
+      <c r="L313" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="M313" s="42" t="s">
+        <v>493</v>
+      </c>
+      <c r="N313" s="43" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="44.05" outlineLevel="0" r="314" s="43">
+      <c r="A314" s="50"/>
+      <c r="B314" s="56" t="s">
+        <v>494</v>
+      </c>
+      <c r="C314" s="58" t="s">
+        <v>279</v>
+      </c>
+      <c r="D314" s="20"/>
+      <c r="E314" s="20"/>
+      <c r="F314" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G314" s="51" t="inlineStr">
+        <f aca="true">NOW()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H314" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I314" s="42" t="s">
+        <v>495</v>
+      </c>
+      <c r="J314" s="40"/>
+      <c r="K314" s="40"/>
+      <c r="L314" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="M314" s="42"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="315" s="43">
+      <c r="A315" s="50"/>
+      <c r="B315" s="56" t="s">
+        <v>496</v>
+      </c>
+      <c r="C315" s="58" t="s">
+        <v>279</v>
+      </c>
+      <c r="D315" s="20"/>
+      <c r="E315" s="20"/>
+      <c r="F315" s="40"/>
+      <c r="G315" s="40"/>
+      <c r="H315" s="52"/>
+      <c r="I315" s="42"/>
+      <c r="J315" s="40"/>
+      <c r="K315" s="40"/>
+      <c r="L315" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="M315" s="42"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="316">
+      <c r="F316" s="16"/>
+      <c r="G316" s="16"/>
+      <c r="H316" s="18"/>
+      <c r="I316" s="19"/>
+      <c r="J316" s="16"/>
+      <c r="K316" s="16"/>
+      <c r="L316" s="18"/>
+      <c r="M316" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="317">
+      <c r="F317" s="16"/>
+      <c r="G317" s="16"/>
+      <c r="H317" s="18"/>
+      <c r="I317" s="19"/>
+      <c r="J317" s="16"/>
+      <c r="K317" s="16"/>
+      <c r="L317" s="18"/>
+      <c r="M317" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="318">
+      <c r="F318" s="16"/>
+      <c r="G318" s="16"/>
+      <c r="H318" s="18"/>
+      <c r="I318" s="19"/>
+      <c r="J318" s="16"/>
+      <c r="K318" s="16"/>
+      <c r="L318" s="18"/>
+      <c r="M318" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="319">
+      <c r="F319" s="16"/>
+      <c r="G319" s="16"/>
+      <c r="H319" s="18"/>
+      <c r="I319" s="19"/>
+      <c r="J319" s="16"/>
+      <c r="K319" s="16"/>
+      <c r="L319" s="18"/>
+      <c r="M319" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="320">
+      <c r="A320" s="22"/>
+      <c r="B320" s="23"/>
+      <c r="C320" s="23"/>
+      <c r="D320" s="23"/>
+      <c r="E320" s="23"/>
+      <c r="F320" s="66"/>
+      <c r="G320" s="66"/>
+      <c r="H320" s="26"/>
+      <c r="I320" s="27"/>
+      <c r="J320" s="66"/>
+      <c r="K320" s="66"/>
+      <c r="L320" s="26"/>
+      <c r="M320" s="27"/>
+      <c r="N320" s="28"/>
+      <c r="O320" s="28"/>
+      <c r="P320" s="28"/>
+      <c r="Q320" s="28"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="321">
+      <c r="A321" s="22"/>
+      <c r="B321" s="23"/>
+      <c r="C321" s="23"/>
+      <c r="D321" s="23"/>
+      <c r="E321" s="23"/>
+      <c r="F321" s="67"/>
+      <c r="G321" s="67"/>
+      <c r="H321" s="68"/>
+      <c r="I321" s="27"/>
+      <c r="J321" s="67"/>
+      <c r="K321" s="67"/>
+      <c r="L321" s="68"/>
+      <c r="M321" s="27"/>
+      <c r="N321" s="28"/>
+      <c r="O321" s="28"/>
+      <c r="P321" s="28"/>
+      <c r="Q321" s="28"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="322">
+      <c r="A322" s="22"/>
+      <c r="B322" s="23"/>
+      <c r="C322" s="23"/>
+      <c r="D322" s="23"/>
+      <c r="E322" s="23"/>
+      <c r="F322" s="67"/>
+      <c r="G322" s="67"/>
+      <c r="H322" s="68"/>
+      <c r="I322" s="27"/>
+      <c r="J322" s="67"/>
+      <c r="K322" s="67"/>
+      <c r="L322" s="68"/>
+      <c r="M322" s="27"/>
+      <c r="N322" s="28"/>
+      <c r="O322" s="28"/>
+      <c r="P322" s="28"/>
+      <c r="Q322" s="28"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="323">
+      <c r="A323" s="22"/>
+      <c r="B323" s="23"/>
+      <c r="C323" s="23"/>
+      <c r="D323" s="23"/>
+      <c r="E323" s="23"/>
+      <c r="F323" s="67"/>
+      <c r="G323" s="67"/>
+      <c r="H323" s="68"/>
+      <c r="I323" s="27"/>
+      <c r="J323" s="67"/>
+      <c r="K323" s="67"/>
+      <c r="L323" s="68"/>
+      <c r="M323" s="27"/>
+      <c r="N323" s="28"/>
+      <c r="O323" s="28"/>
+      <c r="P323" s="28"/>
+      <c r="Q323" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7583,7 +9393,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72156862745098"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added test cases for the specific fields
git-svn-id: https://ark-informatics.googlecode.com/svn/ARK/trunk@8117 2beaffb7-5388-1629-0768-26d37724f1fc
</commit_message>
<xml_diff>
--- a/usefulTools/UAT_FutureRequests.xlsx
+++ b/usefulTools/UAT_FutureRequests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="549">
   <si>
     <t>Result coding: 1 = Pass (full functionality with no unexpected errors), 0 = Fail (lack of required functionality or reproducible error during testing), 9 = Conditional (partial functionality, error during testing which cannot be reproduced, poor user experience or other constraints) X = Functionality which is desirable for future iterations of the system. these items are not necessary for user acceptance of this version of the system</t>
   </si>
@@ -1071,6 +1071,9 @@
     <t>if we enter it, we want to be able to search it - lisa's catchphrase.  We will analyse and test this for the next realease when Data Extraction is due</t>
   </si>
   <si>
+    <t>DEMOGRAPHIC/ADDRESS/PHONE/PERSON FIELDS</t>
+  </si>
+  <si>
     <t>A user with sufficient access can extract the field "First Name"</t>
   </si>
   <si>
@@ -1323,6 +1326,165 @@
     <t>A user with sufficient access can filter on the field "Address Source"</t>
   </si>
   <si>
+    <t>BIOSPECIMEN FIELDS</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field BiospecimenUID</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Sample Type"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Sample Date"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Sample Time"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Processed Date"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Processed Time"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Quantity</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Concentration</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Purity</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Site</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Freezer</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Rack</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Box</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Column</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Row</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Stored In"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Grade</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Comments</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Unit</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field "Treatment Type"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Quality</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Anticoagulant</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Status</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Protocol</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Amount</t>
+  </si>
+  <si>
+    <t>public_field_name</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field BiospecimenUID</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Sample Type"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Sample Date"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Sample Time"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Processed Date"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Processed Time"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field Quantity</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field Concentration</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field Purity</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Stored In"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field Grade</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field Comments</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field Unit</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field "Treatment Type"</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field Quality</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field Anticoagulant</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field Status</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field Protocol</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field Amount</t>
+  </si>
+  <si>
+    <t>BIOCOLLECTION FIELDS</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Name</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Collection UID</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract the field Collection Date</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field Name</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field Collection UID</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can filter on the field Collection Date</t>
+  </si>
+  <si>
     <t>A user with sufficient access can search data for all custom fields entered against a subject.</t>
   </si>
   <si>
@@ -1344,16 +1506,10 @@
     <t>A user with sufficient access can search data for all custom fields entered against a biospecimen.</t>
   </si>
   <si>
-    <t>A user with sufficient access can search data for all fields for a transaction.</t>
-  </si>
-  <si>
-    <t>A user with sufficient access can search data for all fields for a study or substudy.</t>
-  </si>
-  <si>
-    <t>A user with sufficient access can search data for all custom fields entered against a study or substudy.</t>
-  </si>
-  <si>
-    <t>A user with sufficient access can search data for all fields for an inventory object (freezer, site, etc).</t>
+    <t>A user with sufficient access can search data for all fields for a study or substudy.???? perhaps this can go on the study search screen....there really isn't going to be more than 2 studies for most people....sounds excessive to have to search all of this?</t>
+  </si>
+  <si>
+    <t>A user with sufficient access can extract data for all fields for an inventory object (freezer, site, etc).</t>
   </si>
   <si>
     <t>A user with sufficient access can search data for all custom fields entered against an inventory object (freezer, site, etc).</t>
@@ -1715,7 +1871,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
@@ -1940,6 +2096,7 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="2" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
     </xf>
@@ -2036,10 +2193,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R323"/>
+  <dimension ref="A1:R453"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A265" view="normal" windowProtection="false" workbookViewId="0" zoomScale="54" zoomScaleNormal="54" zoomScalePageLayoutView="100">
-      <selection activeCell="B272" activeCellId="0" pane="topLeft" sqref="B272"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A306" view="normal" windowProtection="false" workbookViewId="0" zoomScale="54" zoomScaleNormal="54" zoomScalePageLayoutView="100">
+      <selection activeCell="B324" activeCellId="0" pane="topLeft" sqref="B324"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -6792,8 +6949,8 @@
         <v>350</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="183">
-      <c r="B183" s="0" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="48.35" outlineLevel="0" r="183">
+      <c r="B183" s="30" t="s">
         <v>351</v>
       </c>
       <c r="C183" s="31"/>
@@ -7178,7 +7335,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="207">
       <c r="B207" s="0" t="s">
-        <v>358</v>
+        <v>375</v>
       </c>
       <c r="C207" s="31"/>
       <c r="D207" s="32"/>
@@ -7194,7 +7351,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="208">
       <c r="B208" s="0" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="C208" s="31"/>
       <c r="D208" s="32"/>
@@ -7914,7 +8071,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="253">
       <c r="B253" s="0" t="s">
-        <v>404</v>
+        <v>420</v>
       </c>
       <c r="C253" s="31"/>
       <c r="D253" s="32"/>
@@ -7930,7 +8087,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="254">
       <c r="B254" s="0" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="C254" s="31"/>
       <c r="D254" s="32"/>
@@ -8169,7 +8326,9 @@
       <c r="M268" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="269">
-      <c r="B269" s="0"/>
+      <c r="B269" s="0" t="s">
+        <v>435</v>
+      </c>
       <c r="C269" s="31"/>
       <c r="D269" s="32"/>
       <c r="E269" s="32"/>
@@ -8183,7 +8342,9 @@
       <c r="M269" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="270">
-      <c r="B270" s="0"/>
+      <c r="B270" s="0" t="s">
+        <v>436</v>
+      </c>
       <c r="C270" s="31"/>
       <c r="D270" s="32"/>
       <c r="E270" s="32"/>
@@ -8211,7 +8372,9 @@
       <c r="M271" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="272">
-      <c r="B272" s="0"/>
+      <c r="B272" s="0" t="s">
+        <v>437</v>
+      </c>
       <c r="C272" s="31"/>
       <c r="D272" s="32"/>
       <c r="E272" s="32"/>
@@ -8225,7 +8388,9 @@
       <c r="M272" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="273">
-      <c r="B273" s="30"/>
+      <c r="B273" s="0" t="s">
+        <v>438</v>
+      </c>
       <c r="C273" s="31"/>
       <c r="D273" s="32"/>
       <c r="E273" s="32"/>
@@ -8239,7 +8404,9 @@
       <c r="M273" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="274">
-      <c r="B274" s="30"/>
+      <c r="B274" s="0" t="s">
+        <v>439</v>
+      </c>
       <c r="C274" s="31"/>
       <c r="D274" s="32"/>
       <c r="E274" s="32"/>
@@ -8253,7 +8420,9 @@
       <c r="M274" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="275">
-      <c r="B275" s="30"/>
+      <c r="B275" s="0" t="s">
+        <v>440</v>
+      </c>
       <c r="C275" s="31"/>
       <c r="D275" s="32"/>
       <c r="E275" s="32"/>
@@ -8267,7 +8436,9 @@
       <c r="M275" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="276">
-      <c r="B276" s="30"/>
+      <c r="B276" s="0" t="s">
+        <v>441</v>
+      </c>
       <c r="C276" s="31"/>
       <c r="D276" s="32"/>
       <c r="E276" s="32"/>
@@ -8281,7 +8452,9 @@
       <c r="M276" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="277">
-      <c r="B277" s="30"/>
+      <c r="B277" s="0" t="s">
+        <v>442</v>
+      </c>
       <c r="C277" s="31"/>
       <c r="D277" s="32"/>
       <c r="E277" s="32"/>
@@ -8295,7 +8468,9 @@
       <c r="M277" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="278">
-      <c r="B278" s="30"/>
+      <c r="B278" s="0" t="s">
+        <v>443</v>
+      </c>
       <c r="C278" s="31"/>
       <c r="D278" s="32"/>
       <c r="E278" s="32"/>
@@ -8308,9 +8483,10 @@
       <c r="L278" s="18"/>
       <c r="M278" s="19"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="279" s="65">
-      <c r="A279" s="63"/>
-      <c r="B279" s="30"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="279">
+      <c r="B279" s="0" t="s">
+        <v>444</v>
+      </c>
       <c r="C279" s="31"/>
       <c r="D279" s="32"/>
       <c r="E279" s="32"/>
@@ -8322,12 +8498,11 @@
       <c r="K279" s="16"/>
       <c r="L279" s="18"/>
       <c r="M279" s="19"/>
-      <c r="N279" s="64"/>
-      <c r="O279" s="64"/>
-      <c r="P279" s="64"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="280">
-      <c r="B280" s="30"/>
+      <c r="B280" s="0" t="s">
+        <v>445</v>
+      </c>
       <c r="C280" s="31"/>
       <c r="D280" s="32"/>
       <c r="E280" s="32"/>
@@ -8340,315 +8515,205 @@
       <c r="L280" s="18"/>
       <c r="M280" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.5" outlineLevel="0" r="281">
-      <c r="B281" s="30" t="s">
-        <v>435</v>
-      </c>
-      <c r="C281" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D281" s="32" t="s">
-        <v>436</v>
-      </c>
-      <c r="E281" s="32" t="s">
-        <v>437</v>
-      </c>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="281">
+      <c r="B281" s="0" t="s">
+        <v>446</v>
+      </c>
+      <c r="C281" s="31"/>
+      <c r="D281" s="32"/>
+      <c r="E281" s="32"/>
       <c r="F281" s="16"/>
       <c r="G281" s="16"/>
       <c r="H281" s="18"/>
       <c r="I281" s="19"/>
       <c r="J281" s="16"/>
       <c r="K281" s="16"/>
-      <c r="L281" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M281" s="19" t="s">
-        <v>350</v>
-      </c>
+      <c r="L281" s="18"/>
+      <c r="M281" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="282">
-      <c r="B282" s="30" t="s">
-        <v>438</v>
-      </c>
-      <c r="C282" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D282" s="32" t="s">
-        <v>348</v>
-      </c>
-      <c r="E282" s="32" t="s">
-        <v>349</v>
-      </c>
+      <c r="B282" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="C282" s="31"/>
+      <c r="D282" s="32"/>
+      <c r="E282" s="32"/>
       <c r="F282" s="16"/>
       <c r="G282" s="16"/>
       <c r="H282" s="18"/>
       <c r="I282" s="19"/>
       <c r="J282" s="16"/>
       <c r="K282" s="16"/>
-      <c r="L282" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M282" s="19" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.5" outlineLevel="0" r="283">
-      <c r="B283" s="30" t="s">
-        <v>439</v>
-      </c>
-      <c r="C283" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D283" s="32" t="s">
-        <v>436</v>
-      </c>
-      <c r="E283" s="32" t="s">
-        <v>437</v>
-      </c>
+      <c r="L282" s="18"/>
+      <c r="M282" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="283">
+      <c r="B283" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="C283" s="31"/>
+      <c r="D283" s="32"/>
+      <c r="E283" s="32"/>
       <c r="F283" s="16"/>
       <c r="G283" s="16"/>
       <c r="H283" s="18"/>
       <c r="I283" s="19"/>
       <c r="J283" s="16"/>
       <c r="K283" s="16"/>
-      <c r="L283" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M283" s="19" t="s">
-        <v>350</v>
-      </c>
+      <c r="L283" s="18"/>
+      <c r="M283" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="284">
-      <c r="B284" s="30" t="s">
-        <v>440</v>
-      </c>
-      <c r="C284" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D284" s="32" t="s">
-        <v>348</v>
-      </c>
-      <c r="E284" s="32" t="s">
-        <v>349</v>
-      </c>
+      <c r="B284" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="C284" s="31"/>
+      <c r="D284" s="32"/>
+      <c r="E284" s="32"/>
       <c r="F284" s="16"/>
       <c r="G284" s="16"/>
       <c r="H284" s="18"/>
       <c r="I284" s="19"/>
       <c r="J284" s="16"/>
       <c r="K284" s="16"/>
-      <c r="L284" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M284" s="19" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.5" outlineLevel="0" r="285">
-      <c r="B285" s="30" t="s">
-        <v>441</v>
-      </c>
-      <c r="C285" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D285" s="32" t="s">
-        <v>436</v>
-      </c>
-      <c r="E285" s="32" t="s">
-        <v>437</v>
-      </c>
+      <c r="L284" s="18"/>
+      <c r="M284" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="285">
+      <c r="B285" s="0" t="s">
+        <v>450</v>
+      </c>
+      <c r="C285" s="31"/>
+      <c r="D285" s="32"/>
+      <c r="E285" s="32"/>
       <c r="F285" s="16"/>
       <c r="G285" s="16"/>
       <c r="H285" s="18"/>
       <c r="I285" s="19"/>
       <c r="J285" s="16"/>
       <c r="K285" s="16"/>
-      <c r="L285" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M285" s="19" t="s">
-        <v>350</v>
-      </c>
+      <c r="L285" s="18"/>
+      <c r="M285" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="286">
-      <c r="B286" s="30" t="s">
-        <v>442</v>
-      </c>
-      <c r="C286" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D286" s="32" t="s">
-        <v>348</v>
-      </c>
-      <c r="E286" s="32" t="s">
-        <v>349</v>
-      </c>
+      <c r="B286" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="C286" s="31"/>
+      <c r="D286" s="32"/>
+      <c r="E286" s="32"/>
       <c r="F286" s="16"/>
       <c r="G286" s="16"/>
       <c r="H286" s="18"/>
       <c r="I286" s="19"/>
       <c r="J286" s="16"/>
       <c r="K286" s="16"/>
-      <c r="L286" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M286" s="19" t="s">
-        <v>350</v>
-      </c>
+      <c r="L286" s="18"/>
+      <c r="M286" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="287">
-      <c r="B287" s="30" t="s">
-        <v>443</v>
-      </c>
-      <c r="C287" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D287" s="32" t="s">
-        <v>348</v>
-      </c>
-      <c r="E287" s="32" t="s">
-        <v>349</v>
-      </c>
+      <c r="B287" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="C287" s="31"/>
+      <c r="D287" s="32"/>
+      <c r="E287" s="32"/>
       <c r="F287" s="16"/>
       <c r="G287" s="16"/>
       <c r="H287" s="18"/>
       <c r="I287" s="19"/>
       <c r="J287" s="16"/>
       <c r="K287" s="16"/>
-      <c r="L287" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M287" s="19" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.5" outlineLevel="0" r="288">
-      <c r="B288" s="30" t="s">
-        <v>444</v>
-      </c>
-      <c r="C288" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D288" s="32" t="s">
-        <v>436</v>
-      </c>
-      <c r="E288" s="32" t="s">
-        <v>437</v>
-      </c>
+      <c r="L287" s="18"/>
+      <c r="M287" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="288">
+      <c r="B288" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="C288" s="31"/>
+      <c r="D288" s="32"/>
+      <c r="E288" s="32"/>
       <c r="F288" s="16"/>
       <c r="G288" s="16"/>
       <c r="H288" s="18"/>
       <c r="I288" s="19"/>
       <c r="J288" s="16"/>
       <c r="K288" s="16"/>
-      <c r="L288" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M288" s="19" t="s">
-        <v>350</v>
-      </c>
+      <c r="L288" s="18"/>
+      <c r="M288" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="289">
-      <c r="B289" s="30" t="s">
-        <v>445</v>
-      </c>
-      <c r="C289" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D289" s="32" t="s">
-        <v>348</v>
-      </c>
-      <c r="E289" s="32" t="s">
-        <v>349</v>
-      </c>
+      <c r="B289" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="C289" s="31"/>
+      <c r="D289" s="32"/>
+      <c r="E289" s="32"/>
       <c r="F289" s="16"/>
       <c r="G289" s="16"/>
       <c r="H289" s="18"/>
       <c r="I289" s="19"/>
       <c r="J289" s="16"/>
       <c r="K289" s="16"/>
-      <c r="L289" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M289" s="19" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="53.25" outlineLevel="0" r="290">
-      <c r="B290" s="30" t="s">
-        <v>446</v>
-      </c>
-      <c r="C290" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D290" s="32" t="s">
-        <v>436</v>
-      </c>
-      <c r="E290" s="32" t="s">
-        <v>437</v>
-      </c>
+      <c r="L289" s="18"/>
+      <c r="M289" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="290">
+      <c r="B290" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="C290" s="31"/>
+      <c r="D290" s="32"/>
+      <c r="E290" s="32"/>
       <c r="F290" s="16"/>
       <c r="G290" s="16"/>
       <c r="H290" s="18"/>
       <c r="I290" s="19"/>
       <c r="J290" s="16"/>
       <c r="K290" s="16"/>
-      <c r="L290" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M290" s="19" t="s">
-        <v>350</v>
-      </c>
+      <c r="L290" s="18"/>
+      <c r="M290" s="19"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="291">
-      <c r="B291" s="30" t="s">
-        <v>447</v>
-      </c>
-      <c r="C291" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D291" s="32" t="s">
-        <v>448</v>
-      </c>
-      <c r="E291" s="32" t="s">
-        <v>449</v>
-      </c>
+      <c r="B291" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="C291" s="31"/>
+      <c r="D291" s="32"/>
+      <c r="E291" s="32"/>
       <c r="F291" s="16"/>
       <c r="G291" s="16"/>
       <c r="H291" s="18"/>
       <c r="I291" s="19"/>
       <c r="J291" s="16"/>
       <c r="K291" s="16"/>
-      <c r="L291" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M291" s="19" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="292">
-      <c r="A292" s="22"/>
-      <c r="B292" s="23"/>
-      <c r="C292" s="23"/>
-      <c r="D292" s="23"/>
-      <c r="E292" s="24"/>
-      <c r="F292" s="60"/>
-      <c r="G292" s="60"/>
-      <c r="H292" s="61"/>
-      <c r="I292" s="62"/>
-      <c r="J292" s="60"/>
-      <c r="K292" s="60"/>
-      <c r="L292" s="61"/>
-      <c r="M292" s="62"/>
-      <c r="N292" s="28"/>
-      <c r="O292" s="28"/>
-      <c r="P292" s="28"/>
-      <c r="Q292" s="28"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="293">
-      <c r="B293" s="15" t="s">
-        <v>450</v>
-      </c>
+      <c r="L291" s="18"/>
+      <c r="M291" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="292">
+      <c r="B292" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="C292" s="31"/>
+      <c r="D292" s="32"/>
+      <c r="E292" s="32"/>
+      <c r="F292" s="16"/>
+      <c r="G292" s="16"/>
+      <c r="H292" s="18"/>
+      <c r="I292" s="19"/>
+      <c r="J292" s="16"/>
+      <c r="K292" s="16"/>
+      <c r="L292" s="18"/>
+      <c r="M292" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="293">
+      <c r="B293" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="C293" s="31"/>
+      <c r="D293" s="32"/>
+      <c r="E293" s="32"/>
       <c r="F293" s="16"/>
       <c r="G293" s="16"/>
       <c r="H293" s="18"/>
@@ -8658,281 +8723,173 @@
       <c r="L293" s="18"/>
       <c r="M293" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="294">
-      <c r="B294" s="30" t="s">
-        <v>451</v>
-      </c>
-      <c r="C294" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D294" s="32" t="s">
-        <v>452</v>
-      </c>
-      <c r="E294" s="32" t="s">
-        <v>453</v>
-      </c>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="294">
+      <c r="B294" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="C294" s="31"/>
+      <c r="D294" s="32"/>
+      <c r="E294" s="32"/>
       <c r="F294" s="16"/>
       <c r="G294" s="16"/>
       <c r="H294" s="18"/>
-      <c r="I294" s="19" t="s">
-        <v>454</v>
-      </c>
+      <c r="I294" s="19"/>
       <c r="J294" s="16"/>
       <c r="K294" s="16"/>
-      <c r="L294" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M294" s="19" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="295">
-      <c r="B295" s="30" t="s">
-        <v>455</v>
-      </c>
-      <c r="C295" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D295" s="32" t="s">
-        <v>456</v>
-      </c>
-      <c r="E295" s="32" t="s">
-        <v>457</v>
-      </c>
+      <c r="L294" s="18"/>
+      <c r="M294" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="295">
+      <c r="B295" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="C295" s="31"/>
+      <c r="D295" s="32"/>
+      <c r="E295" s="32"/>
       <c r="F295" s="16"/>
       <c r="G295" s="16"/>
       <c r="H295" s="18"/>
-      <c r="I295" s="19" t="s">
-        <v>454</v>
-      </c>
+      <c r="I295" s="19"/>
       <c r="J295" s="16"/>
       <c r="K295" s="16"/>
-      <c r="L295" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M295" s="19" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="296">
-      <c r="B296" s="30" t="s">
-        <v>458</v>
-      </c>
-      <c r="C296" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D296" s="32" t="s">
-        <v>459</v>
-      </c>
-      <c r="E296" s="32" t="s">
-        <v>460</v>
-      </c>
+      <c r="L295" s="18"/>
+      <c r="M295" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="296">
+      <c r="B296" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="C296" s="31"/>
+      <c r="D296" s="32"/>
+      <c r="E296" s="32"/>
       <c r="F296" s="16"/>
       <c r="G296" s="16"/>
       <c r="H296" s="18"/>
-      <c r="I296" s="19" t="s">
-        <v>454</v>
-      </c>
+      <c r="I296" s="19"/>
       <c r="J296" s="16"/>
       <c r="K296" s="16"/>
-      <c r="L296" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M296" s="19" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="297">
-      <c r="B297" s="30" t="s">
-        <v>461</v>
-      </c>
-      <c r="C297" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D297" s="32" t="s">
+      <c r="L296" s="18"/>
+      <c r="M296" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="297">
+      <c r="B297" s="0" t="s">
         <v>462</v>
       </c>
-      <c r="E297" s="32" t="s">
-        <v>463</v>
-      </c>
+      <c r="C297" s="31"/>
+      <c r="D297" s="32"/>
+      <c r="E297" s="32"/>
       <c r="F297" s="16"/>
       <c r="G297" s="16"/>
       <c r="H297" s="18"/>
-      <c r="I297" s="19" t="s">
-        <v>454</v>
-      </c>
+      <c r="I297" s="19"/>
       <c r="J297" s="16"/>
       <c r="K297" s="16"/>
-      <c r="L297" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M297" s="19" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="298">
-      <c r="B298" s="30" t="s">
-        <v>464</v>
-      </c>
-      <c r="C298" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D298" s="32" t="s">
-        <v>465</v>
-      </c>
-      <c r="E298" s="32" t="s">
-        <v>466</v>
-      </c>
+      <c r="L297" s="18"/>
+      <c r="M297" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="298">
+      <c r="B298" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="C298" s="31"/>
+      <c r="D298" s="32"/>
+      <c r="E298" s="32"/>
       <c r="F298" s="16"/>
       <c r="G298" s="16"/>
       <c r="H298" s="18"/>
-      <c r="I298" s="19" t="s">
-        <v>454</v>
-      </c>
+      <c r="I298" s="19"/>
       <c r="J298" s="16"/>
       <c r="K298" s="16"/>
-      <c r="L298" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M298" s="19" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="299">
-      <c r="B299" s="30" t="s">
-        <v>467</v>
-      </c>
-      <c r="C299" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D299" s="32" t="s">
-        <v>468</v>
-      </c>
-      <c r="E299" s="32" t="s">
-        <v>469</v>
-      </c>
+      <c r="L298" s="18"/>
+      <c r="M298" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="299">
+      <c r="B299" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="C299" s="31"/>
+      <c r="D299" s="32"/>
+      <c r="E299" s="32"/>
       <c r="F299" s="16"/>
       <c r="G299" s="16"/>
       <c r="H299" s="18"/>
-      <c r="I299" s="19" t="s">
-        <v>454</v>
-      </c>
+      <c r="I299" s="19"/>
       <c r="J299" s="16"/>
       <c r="K299" s="16"/>
-      <c r="L299" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M299" s="19" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="300">
-      <c r="B300" s="30" t="s">
-        <v>470</v>
-      </c>
-      <c r="C300" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D300" s="32" t="s">
-        <v>471</v>
-      </c>
-      <c r="E300" s="32" t="s">
-        <v>472</v>
-      </c>
+      <c r="L299" s="18"/>
+      <c r="M299" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="300">
+      <c r="B300" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="C300" s="31"/>
+      <c r="D300" s="32"/>
+      <c r="E300" s="32"/>
       <c r="F300" s="16"/>
       <c r="G300" s="16"/>
       <c r="H300" s="18"/>
-      <c r="I300" s="35" t="s">
-        <v>34</v>
-      </c>
+      <c r="I300" s="19"/>
       <c r="J300" s="16"/>
       <c r="K300" s="16"/>
-      <c r="L300" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M300" s="35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45" outlineLevel="0" r="301">
-      <c r="B301" s="30" t="s">
-        <v>473</v>
-      </c>
-      <c r="C301" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D301" s="32" t="s">
-        <v>474</v>
-      </c>
-      <c r="E301" s="32" t="s">
-        <v>475</v>
-      </c>
+      <c r="L300" s="18"/>
+      <c r="M300" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="301">
+      <c r="B301" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="C301" s="31"/>
+      <c r="D301" s="32"/>
+      <c r="E301" s="32"/>
       <c r="F301" s="16"/>
       <c r="G301" s="16"/>
       <c r="H301" s="18"/>
-      <c r="I301" s="19" t="s">
-        <v>476</v>
-      </c>
+      <c r="I301" s="19"/>
       <c r="J301" s="16"/>
       <c r="K301" s="16"/>
-      <c r="L301" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M301" s="19" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45.75" outlineLevel="0" r="302">
-      <c r="B302" s="30" t="s">
-        <v>477</v>
-      </c>
-      <c r="C302" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="D302" s="32" t="s">
-        <v>478</v>
-      </c>
-      <c r="E302" s="32" t="s">
-        <v>479</v>
-      </c>
+      <c r="L301" s="18"/>
+      <c r="M301" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="302">
+      <c r="B302" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="C302" s="31"/>
+      <c r="D302" s="32"/>
+      <c r="E302" s="32"/>
       <c r="F302" s="16"/>
       <c r="G302" s="16"/>
       <c r="H302" s="18"/>
-      <c r="I302" s="19" t="s">
-        <v>476</v>
-      </c>
+      <c r="I302" s="19"/>
       <c r="J302" s="16"/>
       <c r="K302" s="16"/>
-      <c r="L302" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="M302" s="19" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="303">
-      <c r="A303" s="22"/>
-      <c r="B303" s="23"/>
-      <c r="C303" s="23"/>
-      <c r="D303" s="23"/>
-      <c r="E303" s="24"/>
-      <c r="F303" s="60"/>
-      <c r="G303" s="60"/>
-      <c r="H303" s="61"/>
-      <c r="I303" s="62"/>
-      <c r="J303" s="60"/>
-      <c r="K303" s="60"/>
-      <c r="L303" s="61"/>
-      <c r="M303" s="62"/>
-      <c r="N303" s="28"/>
-      <c r="O303" s="28"/>
-      <c r="P303" s="28"/>
-      <c r="Q303" s="28"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="304">
-      <c r="B304" s="15" t="s">
-        <v>480</v>
-      </c>
+      <c r="L302" s="18"/>
+      <c r="M302" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="303">
+      <c r="B303" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="C303" s="31"/>
+      <c r="D303" s="32"/>
+      <c r="E303" s="32"/>
+      <c r="F303" s="16"/>
+      <c r="G303" s="16"/>
+      <c r="H303" s="18"/>
+      <c r="I303" s="19"/>
+      <c r="J303" s="16"/>
+      <c r="K303" s="16"/>
+      <c r="L303" s="18"/>
+      <c r="M303" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="304">
+      <c r="B304" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="C304" s="31"/>
+      <c r="D304" s="32"/>
+      <c r="E304" s="32"/>
       <c r="F304" s="16"/>
       <c r="G304" s="16"/>
       <c r="H304" s="18"/>
@@ -8942,154 +8899,93 @@
       <c r="L304" s="18"/>
       <c r="M304" s="19"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="19.2" outlineLevel="0" r="305" s="43">
-      <c r="A305" s="39"/>
-      <c r="B305" s="49" t="s">
-        <v>481</v>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="305">
+      <c r="B305" s="0" t="s">
+        <v>470</v>
       </c>
       <c r="C305" s="31"/>
-      <c r="D305" s="20"/>
-      <c r="E305" s="20"/>
-      <c r="F305" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="G305" s="51" t="inlineStr">
-        <f aca="true">NOW()</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H305" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I305" s="42" t="s">
-        <v>482</v>
-      </c>
-      <c r="J305" s="40"/>
-      <c r="K305" s="40"/>
-      <c r="L305" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="M305" s="42" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24.85" outlineLevel="0" r="306" s="43">
-      <c r="A306" s="39"/>
-      <c r="B306" s="49" t="s">
-        <v>483</v>
+      <c r="D305" s="32"/>
+      <c r="E305" s="32"/>
+      <c r="F305" s="16"/>
+      <c r="G305" s="16"/>
+      <c r="H305" s="18"/>
+      <c r="I305" s="19"/>
+      <c r="J305" s="16"/>
+      <c r="K305" s="16"/>
+      <c r="L305" s="18"/>
+      <c r="M305" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="306">
+      <c r="B306" s="0" t="s">
+        <v>471</v>
       </c>
       <c r="C306" s="31"/>
-      <c r="D306" s="20"/>
-      <c r="E306" s="20"/>
-      <c r="F306" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="G306" s="51" t="inlineStr">
-        <f aca="true">NOW()</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H306" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I306" s="42"/>
-      <c r="J306" s="40"/>
-      <c r="K306" s="40"/>
-      <c r="L306" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="M306" s="42"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="36.15" outlineLevel="0" r="307" s="43">
-      <c r="A307" s="39"/>
-      <c r="B307" s="49" t="s">
-        <v>484</v>
+      <c r="D306" s="32"/>
+      <c r="E306" s="32"/>
+      <c r="F306" s="16"/>
+      <c r="G306" s="16"/>
+      <c r="H306" s="18"/>
+      <c r="I306" s="19"/>
+      <c r="J306" s="16"/>
+      <c r="K306" s="16"/>
+      <c r="L306" s="18"/>
+      <c r="M306" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="307">
+      <c r="B307" s="0" t="s">
+        <v>472</v>
       </c>
       <c r="C307" s="31"/>
-      <c r="D307" s="20"/>
-      <c r="E307" s="20"/>
-      <c r="F307" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="G307" s="51" t="inlineStr">
-        <f aca="true">NOW()</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H307" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="I307" s="42"/>
-      <c r="J307" s="40"/>
-      <c r="K307" s="40"/>
-      <c r="L307" s="52" t="s">
-        <v>33</v>
-      </c>
-      <c r="M307" s="42" t="s">
-        <v>485</v>
-      </c>
-      <c r="N307" s="43" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30.75" outlineLevel="0" r="308" s="43">
-      <c r="A308" s="39"/>
-      <c r="B308" s="49" t="s">
-        <v>486</v>
+      <c r="D307" s="32"/>
+      <c r="E307" s="32"/>
+      <c r="F307" s="16"/>
+      <c r="G307" s="16"/>
+      <c r="H307" s="18"/>
+      <c r="I307" s="19"/>
+      <c r="J307" s="16"/>
+      <c r="K307" s="16"/>
+      <c r="L307" s="18"/>
+      <c r="M307" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="308">
+      <c r="B308" s="0" t="s">
+        <v>473</v>
       </c>
       <c r="C308" s="31"/>
-      <c r="D308" s="20"/>
-      <c r="E308" s="20"/>
-      <c r="F308" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="G308" s="51" t="inlineStr">
-        <f aca="true">NOW()</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H308" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I308" s="42" t="s">
-        <v>487</v>
-      </c>
-      <c r="J308" s="40"/>
-      <c r="K308" s="40"/>
-      <c r="L308" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="M308" s="42" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="309">
-      <c r="A309" s="22"/>
-      <c r="B309" s="23"/>
-      <c r="C309" s="23"/>
-      <c r="D309" s="23"/>
-      <c r="E309" s="24"/>
-      <c r="F309" s="60"/>
-      <c r="G309" s="60"/>
-      <c r="H309" s="61"/>
-      <c r="I309" s="62"/>
-      <c r="J309" s="60"/>
-      <c r="K309" s="60"/>
-      <c r="L309" s="61"/>
-      <c r="M309" s="62"/>
-      <c r="N309" s="28"/>
-      <c r="O309" s="28"/>
-      <c r="P309" s="28"/>
-      <c r="Q309" s="28"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="310">
-      <c r="B310" s="15" t="s">
-        <v>488</v>
-      </c>
+      <c r="D308" s="32"/>
+      <c r="E308" s="32"/>
+      <c r="F308" s="16"/>
+      <c r="G308" s="16"/>
+      <c r="H308" s="18"/>
+      <c r="I308" s="19"/>
+      <c r="J308" s="16"/>
+      <c r="K308" s="16"/>
+      <c r="L308" s="18"/>
+      <c r="M308" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="309">
+      <c r="B309" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="C309" s="31"/>
+      <c r="D309" s="32"/>
+      <c r="E309" s="32"/>
+      <c r="F309" s="16"/>
+      <c r="G309" s="16"/>
+      <c r="H309" s="18"/>
+      <c r="I309" s="19"/>
+      <c r="J309" s="16"/>
+      <c r="K309" s="16"/>
+      <c r="L309" s="18"/>
+      <c r="M309" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="310">
+      <c r="B310" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="C310" s="31"/>
+      <c r="D310" s="32"/>
+      <c r="E310" s="32"/>
       <c r="F310" s="16"/>
       <c r="G310" s="16"/>
       <c r="H310" s="18"/>
@@ -9099,159 +8995,93 @@
       <c r="L310" s="18"/>
       <c r="M310" s="19"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="311" s="43">
-      <c r="A311" s="50"/>
-      <c r="B311" s="56" t="s">
-        <v>489</v>
-      </c>
-      <c r="C311" s="58" t="s">
-        <v>279</v>
-      </c>
-      <c r="D311" s="20"/>
-      <c r="E311" s="20"/>
-      <c r="F311" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="G311" s="51" t="inlineStr">
-        <f aca="true">NOW()</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H311" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I311" s="42" t="s">
-        <v>490</v>
-      </c>
-      <c r="J311" s="40"/>
-      <c r="K311" s="40"/>
-      <c r="L311" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="M311" s="42"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="312" s="43">
-      <c r="A312" s="50"/>
-      <c r="B312" s="56" t="s">
-        <v>491</v>
-      </c>
-      <c r="C312" s="58" t="s">
-        <v>279</v>
-      </c>
-      <c r="D312" s="20"/>
-      <c r="E312" s="20"/>
-      <c r="F312" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="G312" s="51" t="inlineStr">
-        <f aca="true">NOW()</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H312" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I312" s="42" t="s">
-        <v>490</v>
-      </c>
-      <c r="J312" s="40"/>
-      <c r="K312" s="40"/>
-      <c r="L312" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="M312" s="42"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="313" s="43">
-      <c r="A313" s="50"/>
-      <c r="B313" s="56" t="s">
-        <v>492</v>
-      </c>
-      <c r="C313" s="58" t="s">
-        <v>279</v>
-      </c>
-      <c r="D313" s="20"/>
-      <c r="E313" s="20"/>
-      <c r="F313" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="G313" s="51" t="inlineStr">
-        <f aca="true">NOW()</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H313" s="52" t="n">
-        <v>9</v>
-      </c>
-      <c r="I313" s="42"/>
-      <c r="J313" s="40"/>
-      <c r="K313" s="40"/>
-      <c r="L313" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="M313" s="42" t="s">
-        <v>493</v>
-      </c>
-      <c r="N313" s="43" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="44.05" outlineLevel="0" r="314" s="43">
-      <c r="A314" s="50"/>
-      <c r="B314" s="56" t="s">
-        <v>494</v>
-      </c>
-      <c r="C314" s="58" t="s">
-        <v>279</v>
-      </c>
-      <c r="D314" s="20"/>
-      <c r="E314" s="20"/>
-      <c r="F314" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="G314" s="51" t="inlineStr">
-        <f aca="true">NOW()</f>
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="H314" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="I314" s="42" t="s">
-        <v>495</v>
-      </c>
-      <c r="J314" s="40"/>
-      <c r="K314" s="40"/>
-      <c r="L314" s="52" t="s">
-        <v>33</v>
-      </c>
-      <c r="M314" s="42"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="315" s="43">
-      <c r="A315" s="50"/>
-      <c r="B315" s="56" t="s">
-        <v>496</v>
-      </c>
-      <c r="C315" s="58" t="s">
-        <v>279</v>
-      </c>
-      <c r="D315" s="20"/>
-      <c r="E315" s="20"/>
-      <c r="F315" s="40"/>
-      <c r="G315" s="40"/>
-      <c r="H315" s="52"/>
-      <c r="I315" s="42"/>
-      <c r="J315" s="40"/>
-      <c r="K315" s="40"/>
-      <c r="L315" s="52" t="s">
-        <v>33</v>
-      </c>
-      <c r="M315" s="42"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="316">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="311">
+      <c r="B311" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="C311" s="31"/>
+      <c r="D311" s="32"/>
+      <c r="E311" s="32"/>
+      <c r="F311" s="16"/>
+      <c r="G311" s="16"/>
+      <c r="H311" s="18"/>
+      <c r="I311" s="19"/>
+      <c r="J311" s="16"/>
+      <c r="K311" s="16"/>
+      <c r="L311" s="18"/>
+      <c r="M311" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="312">
+      <c r="B312" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="C312" s="31"/>
+      <c r="D312" s="32"/>
+      <c r="E312" s="32"/>
+      <c r="F312" s="16"/>
+      <c r="G312" s="16"/>
+      <c r="H312" s="18"/>
+      <c r="I312" s="19"/>
+      <c r="J312" s="16"/>
+      <c r="K312" s="16"/>
+      <c r="L312" s="18"/>
+      <c r="M312" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="313">
+      <c r="B313" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="C313" s="31"/>
+      <c r="D313" s="32"/>
+      <c r="E313" s="32"/>
+      <c r="F313" s="16"/>
+      <c r="G313" s="16"/>
+      <c r="H313" s="18"/>
+      <c r="I313" s="19"/>
+      <c r="J313" s="16"/>
+      <c r="K313" s="16"/>
+      <c r="L313" s="18"/>
+      <c r="M313" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="314">
+      <c r="B314" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="C314" s="31"/>
+      <c r="D314" s="32"/>
+      <c r="E314" s="32"/>
+      <c r="F314" s="16"/>
+      <c r="G314" s="16"/>
+      <c r="H314" s="18"/>
+      <c r="I314" s="19"/>
+      <c r="J314" s="16"/>
+      <c r="K314" s="16"/>
+      <c r="L314" s="18"/>
+      <c r="M314" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="315">
+      <c r="B315" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="C315" s="31"/>
+      <c r="D315" s="32"/>
+      <c r="E315" s="32"/>
+      <c r="F315" s="16"/>
+      <c r="G315" s="16"/>
+      <c r="H315" s="18"/>
+      <c r="I315" s="19"/>
+      <c r="J315" s="16"/>
+      <c r="K315" s="16"/>
+      <c r="L315" s="18"/>
+      <c r="M315" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="316">
+      <c r="B316" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="C316" s="31"/>
+      <c r="D316" s="32"/>
+      <c r="E316" s="32"/>
       <c r="F316" s="16"/>
       <c r="G316" s="16"/>
       <c r="H316" s="18"/>
@@ -9261,7 +9091,13 @@
       <c r="L316" s="18"/>
       <c r="M316" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="317">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="317">
+      <c r="B317" s="63" t="s">
+        <v>482</v>
+      </c>
+      <c r="C317" s="31"/>
+      <c r="D317" s="32"/>
+      <c r="E317" s="32"/>
       <c r="F317" s="16"/>
       <c r="G317" s="16"/>
       <c r="H317" s="18"/>
@@ -9271,7 +9107,13 @@
       <c r="L317" s="18"/>
       <c r="M317" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="318">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="318">
+      <c r="B318" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="C318" s="31"/>
+      <c r="D318" s="32"/>
+      <c r="E318" s="32"/>
       <c r="F318" s="16"/>
       <c r="G318" s="16"/>
       <c r="H318" s="18"/>
@@ -9281,7 +9123,13 @@
       <c r="L318" s="18"/>
       <c r="M318" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="319">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="319">
+      <c r="B319" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="C319" s="31"/>
+      <c r="D319" s="32"/>
+      <c r="E319" s="32"/>
       <c r="F319" s="16"/>
       <c r="G319" s="16"/>
       <c r="H319" s="18"/>
@@ -9291,81 +9139,2298 @@
       <c r="L319" s="18"/>
       <c r="M319" s="19"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="320">
-      <c r="A320" s="22"/>
-      <c r="B320" s="23"/>
-      <c r="C320" s="23"/>
-      <c r="D320" s="23"/>
-      <c r="E320" s="23"/>
-      <c r="F320" s="66"/>
-      <c r="G320" s="66"/>
-      <c r="H320" s="26"/>
-      <c r="I320" s="27"/>
-      <c r="J320" s="66"/>
-      <c r="K320" s="66"/>
-      <c r="L320" s="26"/>
-      <c r="M320" s="27"/>
-      <c r="N320" s="28"/>
-      <c r="O320" s="28"/>
-      <c r="P320" s="28"/>
-      <c r="Q320" s="28"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="321">
-      <c r="A321" s="22"/>
-      <c r="B321" s="23"/>
-      <c r="C321" s="23"/>
-      <c r="D321" s="23"/>
-      <c r="E321" s="23"/>
-      <c r="F321" s="67"/>
-      <c r="G321" s="67"/>
-      <c r="H321" s="68"/>
-      <c r="I321" s="27"/>
-      <c r="J321" s="67"/>
-      <c r="K321" s="67"/>
-      <c r="L321" s="68"/>
-      <c r="M321" s="27"/>
-      <c r="N321" s="28"/>
-      <c r="O321" s="28"/>
-      <c r="P321" s="28"/>
-      <c r="Q321" s="28"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="322">
-      <c r="A322" s="22"/>
-      <c r="B322" s="23"/>
-      <c r="C322" s="23"/>
-      <c r="D322" s="23"/>
-      <c r="E322" s="23"/>
-      <c r="F322" s="67"/>
-      <c r="G322" s="67"/>
-      <c r="H322" s="68"/>
-      <c r="I322" s="27"/>
-      <c r="J322" s="67"/>
-      <c r="K322" s="67"/>
-      <c r="L322" s="68"/>
-      <c r="M322" s="27"/>
-      <c r="N322" s="28"/>
-      <c r="O322" s="28"/>
-      <c r="P322" s="28"/>
-      <c r="Q322" s="28"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="323">
-      <c r="A323" s="22"/>
-      <c r="B323" s="23"/>
-      <c r="C323" s="23"/>
-      <c r="D323" s="23"/>
-      <c r="E323" s="23"/>
-      <c r="F323" s="67"/>
-      <c r="G323" s="67"/>
-      <c r="H323" s="68"/>
-      <c r="I323" s="27"/>
-      <c r="J323" s="67"/>
-      <c r="K323" s="67"/>
-      <c r="L323" s="68"/>
-      <c r="M323" s="27"/>
-      <c r="N323" s="28"/>
-      <c r="O323" s="28"/>
-      <c r="P323" s="28"/>
-      <c r="Q323" s="28"/>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="320">
+      <c r="B320" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="C320" s="31"/>
+      <c r="D320" s="32"/>
+      <c r="E320" s="32"/>
+      <c r="F320" s="16"/>
+      <c r="G320" s="16"/>
+      <c r="H320" s="18"/>
+      <c r="I320" s="19"/>
+      <c r="J320" s="16"/>
+      <c r="K320" s="16"/>
+      <c r="L320" s="18"/>
+      <c r="M320" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="321">
+      <c r="B321" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="C321" s="31"/>
+      <c r="D321" s="32"/>
+      <c r="E321" s="32"/>
+      <c r="F321" s="16"/>
+      <c r="G321" s="16"/>
+      <c r="H321" s="18"/>
+      <c r="I321" s="19"/>
+      <c r="J321" s="16"/>
+      <c r="K321" s="16"/>
+      <c r="L321" s="18"/>
+      <c r="M321" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="322">
+      <c r="B322" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="C322" s="31"/>
+      <c r="D322" s="32"/>
+      <c r="E322" s="32"/>
+      <c r="F322" s="16"/>
+      <c r="G322" s="16"/>
+      <c r="H322" s="18"/>
+      <c r="I322" s="19"/>
+      <c r="J322" s="16"/>
+      <c r="K322" s="16"/>
+      <c r="L322" s="18"/>
+      <c r="M322" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="323">
+      <c r="B323" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="C323" s="31"/>
+      <c r="D323" s="32"/>
+      <c r="E323" s="32"/>
+      <c r="F323" s="16"/>
+      <c r="G323" s="16"/>
+      <c r="H323" s="18"/>
+      <c r="I323" s="19"/>
+      <c r="J323" s="16"/>
+      <c r="K323" s="16"/>
+      <c r="L323" s="18"/>
+      <c r="M323" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="324">
+      <c r="B324" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="C324" s="31"/>
+      <c r="D324" s="32"/>
+      <c r="E324" s="32"/>
+      <c r="F324" s="16"/>
+      <c r="G324" s="16"/>
+      <c r="H324" s="18"/>
+      <c r="I324" s="19"/>
+      <c r="J324" s="16"/>
+      <c r="K324" s="16"/>
+      <c r="L324" s="18"/>
+      <c r="M324" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="325">
+      <c r="B325" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="C325" s="31"/>
+      <c r="D325" s="32"/>
+      <c r="E325" s="32"/>
+      <c r="F325" s="16"/>
+      <c r="G325" s="16"/>
+      <c r="H325" s="18"/>
+      <c r="I325" s="19"/>
+      <c r="J325" s="16"/>
+      <c r="K325" s="16"/>
+      <c r="L325" s="18"/>
+      <c r="M325" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="326">
+      <c r="B326" s="0"/>
+      <c r="C326" s="31"/>
+      <c r="D326" s="32"/>
+      <c r="E326" s="32"/>
+      <c r="F326" s="16"/>
+      <c r="G326" s="16"/>
+      <c r="H326" s="18"/>
+      <c r="I326" s="19"/>
+      <c r="J326" s="16"/>
+      <c r="K326" s="16"/>
+      <c r="L326" s="18"/>
+      <c r="M326" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="327">
+      <c r="B327" s="0"/>
+      <c r="C327" s="31"/>
+      <c r="D327" s="32"/>
+      <c r="E327" s="32"/>
+      <c r="F327" s="16"/>
+      <c r="G327" s="16"/>
+      <c r="H327" s="18"/>
+      <c r="I327" s="19"/>
+      <c r="J327" s="16"/>
+      <c r="K327" s="16"/>
+      <c r="L327" s="18"/>
+      <c r="M327" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="328">
+      <c r="B328" s="0"/>
+      <c r="C328" s="31"/>
+      <c r="D328" s="32"/>
+      <c r="E328" s="32"/>
+      <c r="F328" s="16"/>
+      <c r="G328" s="16"/>
+      <c r="H328" s="18"/>
+      <c r="I328" s="19"/>
+      <c r="J328" s="16"/>
+      <c r="K328" s="16"/>
+      <c r="L328" s="18"/>
+      <c r="M328" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="329">
+      <c r="B329" s="0"/>
+      <c r="C329" s="31"/>
+      <c r="D329" s="32"/>
+      <c r="E329" s="32"/>
+      <c r="F329" s="16"/>
+      <c r="G329" s="16"/>
+      <c r="H329" s="18"/>
+      <c r="I329" s="19"/>
+      <c r="J329" s="16"/>
+      <c r="K329" s="16"/>
+      <c r="L329" s="18"/>
+      <c r="M329" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="330">
+      <c r="B330" s="0"/>
+      <c r="C330" s="31"/>
+      <c r="D330" s="32"/>
+      <c r="E330" s="32"/>
+      <c r="F330" s="16"/>
+      <c r="G330" s="16"/>
+      <c r="H330" s="18"/>
+      <c r="I330" s="19"/>
+      <c r="J330" s="16"/>
+      <c r="K330" s="16"/>
+      <c r="L330" s="18"/>
+      <c r="M330" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="331">
+      <c r="B331" s="0"/>
+      <c r="C331" s="31"/>
+      <c r="D331" s="32"/>
+      <c r="E331" s="32"/>
+      <c r="F331" s="16"/>
+      <c r="G331" s="16"/>
+      <c r="H331" s="18"/>
+      <c r="I331" s="19"/>
+      <c r="J331" s="16"/>
+      <c r="K331" s="16"/>
+      <c r="L331" s="18"/>
+      <c r="M331" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="332">
+      <c r="B332" s="0"/>
+      <c r="C332" s="31"/>
+      <c r="D332" s="32"/>
+      <c r="E332" s="32"/>
+      <c r="F332" s="16"/>
+      <c r="G332" s="16"/>
+      <c r="H332" s="18"/>
+      <c r="I332" s="19"/>
+      <c r="J332" s="16"/>
+      <c r="K332" s="16"/>
+      <c r="L332" s="18"/>
+      <c r="M332" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="333">
+      <c r="B333" s="0"/>
+      <c r="C333" s="31"/>
+      <c r="D333" s="32"/>
+      <c r="E333" s="32"/>
+      <c r="F333" s="16"/>
+      <c r="G333" s="16"/>
+      <c r="H333" s="18"/>
+      <c r="I333" s="19"/>
+      <c r="J333" s="16"/>
+      <c r="K333" s="16"/>
+      <c r="L333" s="18"/>
+      <c r="M333" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="334">
+      <c r="B334" s="0"/>
+      <c r="C334" s="31"/>
+      <c r="D334" s="32"/>
+      <c r="E334" s="32"/>
+      <c r="F334" s="16"/>
+      <c r="G334" s="16"/>
+      <c r="H334" s="18"/>
+      <c r="I334" s="19"/>
+      <c r="J334" s="16"/>
+      <c r="K334" s="16"/>
+      <c r="L334" s="18"/>
+      <c r="M334" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="335">
+      <c r="B335" s="0"/>
+      <c r="C335" s="31"/>
+      <c r="D335" s="32"/>
+      <c r="E335" s="32"/>
+      <c r="F335" s="16"/>
+      <c r="G335" s="16"/>
+      <c r="H335" s="18"/>
+      <c r="I335" s="19"/>
+      <c r="J335" s="16"/>
+      <c r="K335" s="16"/>
+      <c r="L335" s="18"/>
+      <c r="M335" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="336">
+      <c r="B336" s="0"/>
+      <c r="C336" s="31"/>
+      <c r="D336" s="32"/>
+      <c r="E336" s="32"/>
+      <c r="F336" s="16"/>
+      <c r="G336" s="16"/>
+      <c r="H336" s="18"/>
+      <c r="I336" s="19"/>
+      <c r="J336" s="16"/>
+      <c r="K336" s="16"/>
+      <c r="L336" s="18"/>
+      <c r="M336" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="337">
+      <c r="B337" s="0"/>
+      <c r="C337" s="31"/>
+      <c r="D337" s="32"/>
+      <c r="E337" s="32"/>
+      <c r="F337" s="16"/>
+      <c r="G337" s="16"/>
+      <c r="H337" s="18"/>
+      <c r="I337" s="19"/>
+      <c r="J337" s="16"/>
+      <c r="K337" s="16"/>
+      <c r="L337" s="18"/>
+      <c r="M337" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="338">
+      <c r="B338" s="0"/>
+      <c r="C338" s="31"/>
+      <c r="D338" s="32"/>
+      <c r="E338" s="32"/>
+      <c r="F338" s="16"/>
+      <c r="G338" s="16"/>
+      <c r="H338" s="18"/>
+      <c r="I338" s="19"/>
+      <c r="J338" s="16"/>
+      <c r="K338" s="16"/>
+      <c r="L338" s="18"/>
+      <c r="M338" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="339">
+      <c r="B339" s="0"/>
+      <c r="C339" s="31"/>
+      <c r="D339" s="32"/>
+      <c r="E339" s="32"/>
+      <c r="F339" s="16"/>
+      <c r="G339" s="16"/>
+      <c r="H339" s="18"/>
+      <c r="I339" s="19"/>
+      <c r="J339" s="16"/>
+      <c r="K339" s="16"/>
+      <c r="L339" s="18"/>
+      <c r="M339" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="340">
+      <c r="B340" s="0"/>
+      <c r="C340" s="31"/>
+      <c r="D340" s="32"/>
+      <c r="E340" s="32"/>
+      <c r="F340" s="16"/>
+      <c r="G340" s="16"/>
+      <c r="H340" s="18"/>
+      <c r="I340" s="19"/>
+      <c r="J340" s="16"/>
+      <c r="K340" s="16"/>
+      <c r="L340" s="18"/>
+      <c r="M340" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="341">
+      <c r="B341" s="0"/>
+      <c r="C341" s="31"/>
+      <c r="D341" s="32"/>
+      <c r="E341" s="32"/>
+      <c r="F341" s="16"/>
+      <c r="G341" s="16"/>
+      <c r="H341" s="18"/>
+      <c r="I341" s="19"/>
+      <c r="J341" s="16"/>
+      <c r="K341" s="16"/>
+      <c r="L341" s="18"/>
+      <c r="M341" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="342">
+      <c r="B342" s="0"/>
+      <c r="C342" s="31"/>
+      <c r="D342" s="32"/>
+      <c r="E342" s="32"/>
+      <c r="F342" s="16"/>
+      <c r="G342" s="16"/>
+      <c r="H342" s="18"/>
+      <c r="I342" s="19"/>
+      <c r="J342" s="16"/>
+      <c r="K342" s="16"/>
+      <c r="L342" s="18"/>
+      <c r="M342" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="343">
+      <c r="B343" s="0"/>
+      <c r="C343" s="31"/>
+      <c r="D343" s="32"/>
+      <c r="E343" s="32"/>
+      <c r="F343" s="16"/>
+      <c r="G343" s="16"/>
+      <c r="H343" s="18"/>
+      <c r="I343" s="19"/>
+      <c r="J343" s="16"/>
+      <c r="K343" s="16"/>
+      <c r="L343" s="18"/>
+      <c r="M343" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="344">
+      <c r="B344" s="0"/>
+      <c r="C344" s="31"/>
+      <c r="D344" s="32"/>
+      <c r="E344" s="32"/>
+      <c r="F344" s="16"/>
+      <c r="G344" s="16"/>
+      <c r="H344" s="18"/>
+      <c r="I344" s="19"/>
+      <c r="J344" s="16"/>
+      <c r="K344" s="16"/>
+      <c r="L344" s="18"/>
+      <c r="M344" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="345">
+      <c r="B345" s="0"/>
+      <c r="C345" s="31"/>
+      <c r="D345" s="32"/>
+      <c r="E345" s="32"/>
+      <c r="F345" s="16"/>
+      <c r="G345" s="16"/>
+      <c r="H345" s="18"/>
+      <c r="I345" s="19"/>
+      <c r="J345" s="16"/>
+      <c r="K345" s="16"/>
+      <c r="L345" s="18"/>
+      <c r="M345" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="346">
+      <c r="B346" s="0"/>
+      <c r="C346" s="31"/>
+      <c r="D346" s="32"/>
+      <c r="E346" s="32"/>
+      <c r="F346" s="16"/>
+      <c r="G346" s="16"/>
+      <c r="H346" s="18"/>
+      <c r="I346" s="19"/>
+      <c r="J346" s="16"/>
+      <c r="K346" s="16"/>
+      <c r="L346" s="18"/>
+      <c r="M346" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="347">
+      <c r="B347" s="0"/>
+      <c r="C347" s="31"/>
+      <c r="D347" s="32"/>
+      <c r="E347" s="32"/>
+      <c r="F347" s="16"/>
+      <c r="G347" s="16"/>
+      <c r="H347" s="18"/>
+      <c r="I347" s="19"/>
+      <c r="J347" s="16"/>
+      <c r="K347" s="16"/>
+      <c r="L347" s="18"/>
+      <c r="M347" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="348">
+      <c r="B348" s="0"/>
+      <c r="C348" s="31"/>
+      <c r="D348" s="32"/>
+      <c r="E348" s="32"/>
+      <c r="F348" s="16"/>
+      <c r="G348" s="16"/>
+      <c r="H348" s="18"/>
+      <c r="I348" s="19"/>
+      <c r="J348" s="16"/>
+      <c r="K348" s="16"/>
+      <c r="L348" s="18"/>
+      <c r="M348" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="349">
+      <c r="B349" s="0"/>
+      <c r="C349" s="31"/>
+      <c r="D349" s="32"/>
+      <c r="E349" s="32"/>
+      <c r="F349" s="16"/>
+      <c r="G349" s="16"/>
+      <c r="H349" s="18"/>
+      <c r="I349" s="19"/>
+      <c r="J349" s="16"/>
+      <c r="K349" s="16"/>
+      <c r="L349" s="18"/>
+      <c r="M349" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="350">
+      <c r="B350" s="0"/>
+      <c r="C350" s="31"/>
+      <c r="D350" s="32"/>
+      <c r="E350" s="32"/>
+      <c r="F350" s="16"/>
+      <c r="G350" s="16"/>
+      <c r="H350" s="18"/>
+      <c r="I350" s="19"/>
+      <c r="J350" s="16"/>
+      <c r="K350" s="16"/>
+      <c r="L350" s="18"/>
+      <c r="M350" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="351">
+      <c r="B351" s="0"/>
+      <c r="C351" s="31"/>
+      <c r="D351" s="32"/>
+      <c r="E351" s="32"/>
+      <c r="F351" s="16"/>
+      <c r="G351" s="16"/>
+      <c r="H351" s="18"/>
+      <c r="I351" s="19"/>
+      <c r="J351" s="16"/>
+      <c r="K351" s="16"/>
+      <c r="L351" s="18"/>
+      <c r="M351" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="352">
+      <c r="B352" s="0"/>
+      <c r="C352" s="31"/>
+      <c r="D352" s="32"/>
+      <c r="E352" s="32"/>
+      <c r="F352" s="16"/>
+      <c r="G352" s="16"/>
+      <c r="H352" s="18"/>
+      <c r="I352" s="19"/>
+      <c r="J352" s="16"/>
+      <c r="K352" s="16"/>
+      <c r="L352" s="18"/>
+      <c r="M352" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="353">
+      <c r="B353" s="0"/>
+      <c r="C353" s="31"/>
+      <c r="D353" s="32"/>
+      <c r="E353" s="32"/>
+      <c r="F353" s="16"/>
+      <c r="G353" s="16"/>
+      <c r="H353" s="18"/>
+      <c r="I353" s="19"/>
+      <c r="J353" s="16"/>
+      <c r="K353" s="16"/>
+      <c r="L353" s="18"/>
+      <c r="M353" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="354">
+      <c r="B354" s="0"/>
+      <c r="C354" s="31"/>
+      <c r="D354" s="32"/>
+      <c r="E354" s="32"/>
+      <c r="F354" s="16"/>
+      <c r="G354" s="16"/>
+      <c r="H354" s="18"/>
+      <c r="I354" s="19"/>
+      <c r="J354" s="16"/>
+      <c r="K354" s="16"/>
+      <c r="L354" s="18"/>
+      <c r="M354" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="355">
+      <c r="B355" s="0"/>
+      <c r="C355" s="31"/>
+      <c r="D355" s="32"/>
+      <c r="E355" s="32"/>
+      <c r="F355" s="16"/>
+      <c r="G355" s="16"/>
+      <c r="H355" s="18"/>
+      <c r="I355" s="19"/>
+      <c r="J355" s="16"/>
+      <c r="K355" s="16"/>
+      <c r="L355" s="18"/>
+      <c r="M355" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="356">
+      <c r="B356" s="0"/>
+      <c r="C356" s="31"/>
+      <c r="D356" s="32"/>
+      <c r="E356" s="32"/>
+      <c r="F356" s="16"/>
+      <c r="G356" s="16"/>
+      <c r="H356" s="18"/>
+      <c r="I356" s="19"/>
+      <c r="J356" s="16"/>
+      <c r="K356" s="16"/>
+      <c r="L356" s="18"/>
+      <c r="M356" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="357">
+      <c r="B357" s="0"/>
+      <c r="C357" s="31"/>
+      <c r="D357" s="32"/>
+      <c r="E357" s="32"/>
+      <c r="F357" s="16"/>
+      <c r="G357" s="16"/>
+      <c r="H357" s="18"/>
+      <c r="I357" s="19"/>
+      <c r="J357" s="16"/>
+      <c r="K357" s="16"/>
+      <c r="L357" s="18"/>
+      <c r="M357" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="358">
+      <c r="B358" s="0"/>
+      <c r="C358" s="31"/>
+      <c r="D358" s="32"/>
+      <c r="E358" s="32"/>
+      <c r="F358" s="16"/>
+      <c r="G358" s="16"/>
+      <c r="H358" s="18"/>
+      <c r="I358" s="19"/>
+      <c r="J358" s="16"/>
+      <c r="K358" s="16"/>
+      <c r="L358" s="18"/>
+      <c r="M358" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="359">
+      <c r="B359" s="0"/>
+      <c r="C359" s="31"/>
+      <c r="D359" s="32"/>
+      <c r="E359" s="32"/>
+      <c r="F359" s="16"/>
+      <c r="G359" s="16"/>
+      <c r="H359" s="18"/>
+      <c r="I359" s="19"/>
+      <c r="J359" s="16"/>
+      <c r="K359" s="16"/>
+      <c r="L359" s="18"/>
+      <c r="M359" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="360">
+      <c r="B360" s="0"/>
+      <c r="C360" s="31"/>
+      <c r="D360" s="32"/>
+      <c r="E360" s="32"/>
+      <c r="F360" s="16"/>
+      <c r="G360" s="16"/>
+      <c r="H360" s="18"/>
+      <c r="I360" s="19"/>
+      <c r="J360" s="16"/>
+      <c r="K360" s="16"/>
+      <c r="L360" s="18"/>
+      <c r="M360" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="361">
+      <c r="B361" s="0"/>
+      <c r="C361" s="31"/>
+      <c r="D361" s="32"/>
+      <c r="E361" s="32"/>
+      <c r="F361" s="16"/>
+      <c r="G361" s="16"/>
+      <c r="H361" s="18"/>
+      <c r="I361" s="19"/>
+      <c r="J361" s="16"/>
+      <c r="K361" s="16"/>
+      <c r="L361" s="18"/>
+      <c r="M361" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="362">
+      <c r="B362" s="0"/>
+      <c r="C362" s="31"/>
+      <c r="D362" s="32"/>
+      <c r="E362" s="32"/>
+      <c r="F362" s="16"/>
+      <c r="G362" s="16"/>
+      <c r="H362" s="18"/>
+      <c r="I362" s="19"/>
+      <c r="J362" s="16"/>
+      <c r="K362" s="16"/>
+      <c r="L362" s="18"/>
+      <c r="M362" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="363">
+      <c r="B363" s="0"/>
+      <c r="C363" s="31"/>
+      <c r="D363" s="32"/>
+      <c r="E363" s="32"/>
+      <c r="F363" s="16"/>
+      <c r="G363" s="16"/>
+      <c r="H363" s="18"/>
+      <c r="I363" s="19"/>
+      <c r="J363" s="16"/>
+      <c r="K363" s="16"/>
+      <c r="L363" s="18"/>
+      <c r="M363" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="364">
+      <c r="B364" s="0"/>
+      <c r="C364" s="31"/>
+      <c r="D364" s="32"/>
+      <c r="E364" s="32"/>
+      <c r="F364" s="16"/>
+      <c r="G364" s="16"/>
+      <c r="H364" s="18"/>
+      <c r="I364" s="19"/>
+      <c r="J364" s="16"/>
+      <c r="K364" s="16"/>
+      <c r="L364" s="18"/>
+      <c r="M364" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="365">
+      <c r="B365" s="0"/>
+      <c r="C365" s="31"/>
+      <c r="D365" s="32"/>
+      <c r="E365" s="32"/>
+      <c r="F365" s="16"/>
+      <c r="G365" s="16"/>
+      <c r="H365" s="18"/>
+      <c r="I365" s="19"/>
+      <c r="J365" s="16"/>
+      <c r="K365" s="16"/>
+      <c r="L365" s="18"/>
+      <c r="M365" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="366">
+      <c r="B366" s="0"/>
+      <c r="C366" s="31"/>
+      <c r="D366" s="32"/>
+      <c r="E366" s="32"/>
+      <c r="F366" s="16"/>
+      <c r="G366" s="16"/>
+      <c r="H366" s="18"/>
+      <c r="I366" s="19"/>
+      <c r="J366" s="16"/>
+      <c r="K366" s="16"/>
+      <c r="L366" s="18"/>
+      <c r="M366" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="367">
+      <c r="B367" s="0"/>
+      <c r="C367" s="31"/>
+      <c r="D367" s="32"/>
+      <c r="E367" s="32"/>
+      <c r="F367" s="16"/>
+      <c r="G367" s="16"/>
+      <c r="H367" s="18"/>
+      <c r="I367" s="19"/>
+      <c r="J367" s="16"/>
+      <c r="K367" s="16"/>
+      <c r="L367" s="18"/>
+      <c r="M367" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="368">
+      <c r="B368" s="0"/>
+      <c r="C368" s="31"/>
+      <c r="D368" s="32"/>
+      <c r="E368" s="32"/>
+      <c r="F368" s="16"/>
+      <c r="G368" s="16"/>
+      <c r="H368" s="18"/>
+      <c r="I368" s="19"/>
+      <c r="J368" s="16"/>
+      <c r="K368" s="16"/>
+      <c r="L368" s="18"/>
+      <c r="M368" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="369">
+      <c r="B369" s="0"/>
+      <c r="C369" s="31"/>
+      <c r="D369" s="32"/>
+      <c r="E369" s="32"/>
+      <c r="F369" s="16"/>
+      <c r="G369" s="16"/>
+      <c r="H369" s="18"/>
+      <c r="I369" s="19"/>
+      <c r="J369" s="16"/>
+      <c r="K369" s="16"/>
+      <c r="L369" s="18"/>
+      <c r="M369" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="370">
+      <c r="B370" s="0"/>
+      <c r="C370" s="31"/>
+      <c r="D370" s="32"/>
+      <c r="E370" s="32"/>
+      <c r="F370" s="16"/>
+      <c r="G370" s="16"/>
+      <c r="H370" s="18"/>
+      <c r="I370" s="19"/>
+      <c r="J370" s="16"/>
+      <c r="K370" s="16"/>
+      <c r="L370" s="18"/>
+      <c r="M370" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="371">
+      <c r="B371" s="0"/>
+      <c r="C371" s="31"/>
+      <c r="D371" s="32"/>
+      <c r="E371" s="32"/>
+      <c r="F371" s="16"/>
+      <c r="G371" s="16"/>
+      <c r="H371" s="18"/>
+      <c r="I371" s="19"/>
+      <c r="J371" s="16"/>
+      <c r="K371" s="16"/>
+      <c r="L371" s="18"/>
+      <c r="M371" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="372">
+      <c r="B372" s="0"/>
+      <c r="C372" s="31"/>
+      <c r="D372" s="32"/>
+      <c r="E372" s="32"/>
+      <c r="F372" s="16"/>
+      <c r="G372" s="16"/>
+      <c r="H372" s="18"/>
+      <c r="I372" s="19"/>
+      <c r="J372" s="16"/>
+      <c r="K372" s="16"/>
+      <c r="L372" s="18"/>
+      <c r="M372" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="373">
+      <c r="B373" s="0"/>
+      <c r="C373" s="31"/>
+      <c r="D373" s="32"/>
+      <c r="E373" s="32"/>
+      <c r="F373" s="16"/>
+      <c r="G373" s="16"/>
+      <c r="H373" s="18"/>
+      <c r="I373" s="19"/>
+      <c r="J373" s="16"/>
+      <c r="K373" s="16"/>
+      <c r="L373" s="18"/>
+      <c r="M373" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="374">
+      <c r="B374" s="0"/>
+      <c r="C374" s="31"/>
+      <c r="D374" s="32"/>
+      <c r="E374" s="32"/>
+      <c r="F374" s="16"/>
+      <c r="G374" s="16"/>
+      <c r="H374" s="18"/>
+      <c r="I374" s="19"/>
+      <c r="J374" s="16"/>
+      <c r="K374" s="16"/>
+      <c r="L374" s="18"/>
+      <c r="M374" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="375">
+      <c r="B375" s="0"/>
+      <c r="C375" s="31"/>
+      <c r="D375" s="32"/>
+      <c r="E375" s="32"/>
+      <c r="F375" s="16"/>
+      <c r="G375" s="16"/>
+      <c r="H375" s="18"/>
+      <c r="I375" s="19"/>
+      <c r="J375" s="16"/>
+      <c r="K375" s="16"/>
+      <c r="L375" s="18"/>
+      <c r="M375" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="376">
+      <c r="B376" s="0"/>
+      <c r="C376" s="31"/>
+      <c r="D376" s="32"/>
+      <c r="E376" s="32"/>
+      <c r="F376" s="16"/>
+      <c r="G376" s="16"/>
+      <c r="H376" s="18"/>
+      <c r="I376" s="19"/>
+      <c r="J376" s="16"/>
+      <c r="K376" s="16"/>
+      <c r="L376" s="18"/>
+      <c r="M376" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="377">
+      <c r="B377" s="0"/>
+      <c r="C377" s="31"/>
+      <c r="D377" s="32"/>
+      <c r="E377" s="32"/>
+      <c r="F377" s="16"/>
+      <c r="G377" s="16"/>
+      <c r="H377" s="18"/>
+      <c r="I377" s="19"/>
+      <c r="J377" s="16"/>
+      <c r="K377" s="16"/>
+      <c r="L377" s="18"/>
+      <c r="M377" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="378">
+      <c r="B378" s="0"/>
+      <c r="C378" s="31"/>
+      <c r="D378" s="32"/>
+      <c r="E378" s="32"/>
+      <c r="F378" s="16"/>
+      <c r="G378" s="16"/>
+      <c r="H378" s="18"/>
+      <c r="I378" s="19"/>
+      <c r="J378" s="16"/>
+      <c r="K378" s="16"/>
+      <c r="L378" s="18"/>
+      <c r="M378" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="379">
+      <c r="B379" s="0"/>
+      <c r="C379" s="31"/>
+      <c r="D379" s="32"/>
+      <c r="E379" s="32"/>
+      <c r="F379" s="16"/>
+      <c r="G379" s="16"/>
+      <c r="H379" s="18"/>
+      <c r="I379" s="19"/>
+      <c r="J379" s="16"/>
+      <c r="K379" s="16"/>
+      <c r="L379" s="18"/>
+      <c r="M379" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="380">
+      <c r="B380" s="0"/>
+      <c r="C380" s="31"/>
+      <c r="D380" s="32"/>
+      <c r="E380" s="32"/>
+      <c r="F380" s="16"/>
+      <c r="G380" s="16"/>
+      <c r="H380" s="18"/>
+      <c r="I380" s="19"/>
+      <c r="J380" s="16"/>
+      <c r="K380" s="16"/>
+      <c r="L380" s="18"/>
+      <c r="M380" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="381">
+      <c r="B381" s="0"/>
+      <c r="C381" s="31"/>
+      <c r="D381" s="32"/>
+      <c r="E381" s="32"/>
+      <c r="F381" s="16"/>
+      <c r="G381" s="16"/>
+      <c r="H381" s="18"/>
+      <c r="I381" s="19"/>
+      <c r="J381" s="16"/>
+      <c r="K381" s="16"/>
+      <c r="L381" s="18"/>
+      <c r="M381" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="382">
+      <c r="B382" s="0"/>
+      <c r="C382" s="31"/>
+      <c r="D382" s="32"/>
+      <c r="E382" s="32"/>
+      <c r="F382" s="16"/>
+      <c r="G382" s="16"/>
+      <c r="H382" s="18"/>
+      <c r="I382" s="19"/>
+      <c r="J382" s="16"/>
+      <c r="K382" s="16"/>
+      <c r="L382" s="18"/>
+      <c r="M382" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="383">
+      <c r="B383" s="0"/>
+      <c r="C383" s="31"/>
+      <c r="D383" s="32"/>
+      <c r="E383" s="32"/>
+      <c r="F383" s="16"/>
+      <c r="G383" s="16"/>
+      <c r="H383" s="18"/>
+      <c r="I383" s="19"/>
+      <c r="J383" s="16"/>
+      <c r="K383" s="16"/>
+      <c r="L383" s="18"/>
+      <c r="M383" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="384">
+      <c r="B384" s="0"/>
+      <c r="C384" s="31"/>
+      <c r="D384" s="32"/>
+      <c r="E384" s="32"/>
+      <c r="F384" s="16"/>
+      <c r="G384" s="16"/>
+      <c r="H384" s="18"/>
+      <c r="I384" s="19"/>
+      <c r="J384" s="16"/>
+      <c r="K384" s="16"/>
+      <c r="L384" s="18"/>
+      <c r="M384" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="385">
+      <c r="B385" s="0"/>
+      <c r="C385" s="31"/>
+      <c r="D385" s="32"/>
+      <c r="E385" s="32"/>
+      <c r="F385" s="16"/>
+      <c r="G385" s="16"/>
+      <c r="H385" s="18"/>
+      <c r="I385" s="19"/>
+      <c r="J385" s="16"/>
+      <c r="K385" s="16"/>
+      <c r="L385" s="18"/>
+      <c r="M385" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="386">
+      <c r="B386" s="0"/>
+      <c r="C386" s="31"/>
+      <c r="D386" s="32"/>
+      <c r="E386" s="32"/>
+      <c r="F386" s="16"/>
+      <c r="G386" s="16"/>
+      <c r="H386" s="18"/>
+      <c r="I386" s="19"/>
+      <c r="J386" s="16"/>
+      <c r="K386" s="16"/>
+      <c r="L386" s="18"/>
+      <c r="M386" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="387">
+      <c r="B387" s="0"/>
+      <c r="C387" s="31"/>
+      <c r="D387" s="32"/>
+      <c r="E387" s="32"/>
+      <c r="F387" s="16"/>
+      <c r="G387" s="16"/>
+      <c r="H387" s="18"/>
+      <c r="I387" s="19"/>
+      <c r="J387" s="16"/>
+      <c r="K387" s="16"/>
+      <c r="L387" s="18"/>
+      <c r="M387" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="388">
+      <c r="B388" s="0"/>
+      <c r="C388" s="31"/>
+      <c r="D388" s="32"/>
+      <c r="E388" s="32"/>
+      <c r="F388" s="16"/>
+      <c r="G388" s="16"/>
+      <c r="H388" s="18"/>
+      <c r="I388" s="19"/>
+      <c r="J388" s="16"/>
+      <c r="K388" s="16"/>
+      <c r="L388" s="18"/>
+      <c r="M388" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="389">
+      <c r="B389" s="0"/>
+      <c r="C389" s="31"/>
+      <c r="D389" s="32"/>
+      <c r="E389" s="32"/>
+      <c r="F389" s="16"/>
+      <c r="G389" s="16"/>
+      <c r="H389" s="18"/>
+      <c r="I389" s="19"/>
+      <c r="J389" s="16"/>
+      <c r="K389" s="16"/>
+      <c r="L389" s="18"/>
+      <c r="M389" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="390">
+      <c r="B390" s="0"/>
+      <c r="C390" s="31"/>
+      <c r="D390" s="32"/>
+      <c r="E390" s="32"/>
+      <c r="F390" s="16"/>
+      <c r="G390" s="16"/>
+      <c r="H390" s="18"/>
+      <c r="I390" s="19"/>
+      <c r="J390" s="16"/>
+      <c r="K390" s="16"/>
+      <c r="L390" s="18"/>
+      <c r="M390" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="391">
+      <c r="B391" s="0"/>
+      <c r="C391" s="31"/>
+      <c r="D391" s="32"/>
+      <c r="E391" s="32"/>
+      <c r="F391" s="16"/>
+      <c r="G391" s="16"/>
+      <c r="H391" s="18"/>
+      <c r="I391" s="19"/>
+      <c r="J391" s="16"/>
+      <c r="K391" s="16"/>
+      <c r="L391" s="18"/>
+      <c r="M391" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="392">
+      <c r="B392" s="0"/>
+      <c r="C392" s="31"/>
+      <c r="D392" s="32"/>
+      <c r="E392" s="32"/>
+      <c r="F392" s="16"/>
+      <c r="G392" s="16"/>
+      <c r="H392" s="18"/>
+      <c r="I392" s="19"/>
+      <c r="J392" s="16"/>
+      <c r="K392" s="16"/>
+      <c r="L392" s="18"/>
+      <c r="M392" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="393">
+      <c r="B393" s="0"/>
+      <c r="C393" s="31"/>
+      <c r="D393" s="32"/>
+      <c r="E393" s="32"/>
+      <c r="F393" s="16"/>
+      <c r="G393" s="16"/>
+      <c r="H393" s="18"/>
+      <c r="I393" s="19"/>
+      <c r="J393" s="16"/>
+      <c r="K393" s="16"/>
+      <c r="L393" s="18"/>
+      <c r="M393" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="394">
+      <c r="B394" s="0"/>
+      <c r="C394" s="31"/>
+      <c r="D394" s="32"/>
+      <c r="E394" s="32"/>
+      <c r="F394" s="16"/>
+      <c r="G394" s="16"/>
+      <c r="H394" s="18"/>
+      <c r="I394" s="19"/>
+      <c r="J394" s="16"/>
+      <c r="K394" s="16"/>
+      <c r="L394" s="18"/>
+      <c r="M394" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="395">
+      <c r="B395" s="0"/>
+      <c r="C395" s="31"/>
+      <c r="D395" s="32"/>
+      <c r="E395" s="32"/>
+      <c r="F395" s="16"/>
+      <c r="G395" s="16"/>
+      <c r="H395" s="18"/>
+      <c r="I395" s="19"/>
+      <c r="J395" s="16"/>
+      <c r="K395" s="16"/>
+      <c r="L395" s="18"/>
+      <c r="M395" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="396">
+      <c r="B396" s="0"/>
+      <c r="C396" s="31"/>
+      <c r="D396" s="32"/>
+      <c r="E396" s="32"/>
+      <c r="F396" s="16"/>
+      <c r="G396" s="16"/>
+      <c r="H396" s="18"/>
+      <c r="I396" s="19"/>
+      <c r="J396" s="16"/>
+      <c r="K396" s="16"/>
+      <c r="L396" s="18"/>
+      <c r="M396" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="397">
+      <c r="B397" s="0"/>
+      <c r="C397" s="31"/>
+      <c r="D397" s="32"/>
+      <c r="E397" s="32"/>
+      <c r="F397" s="16"/>
+      <c r="G397" s="16"/>
+      <c r="H397" s="18"/>
+      <c r="I397" s="19"/>
+      <c r="J397" s="16"/>
+      <c r="K397" s="16"/>
+      <c r="L397" s="18"/>
+      <c r="M397" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="398">
+      <c r="B398" s="0"/>
+      <c r="C398" s="31"/>
+      <c r="D398" s="32"/>
+      <c r="E398" s="32"/>
+      <c r="F398" s="16"/>
+      <c r="G398" s="16"/>
+      <c r="H398" s="18"/>
+      <c r="I398" s="19"/>
+      <c r="J398" s="16"/>
+      <c r="K398" s="16"/>
+      <c r="L398" s="18"/>
+      <c r="M398" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="399">
+      <c r="B399" s="0"/>
+      <c r="C399" s="31"/>
+      <c r="D399" s="32"/>
+      <c r="E399" s="32"/>
+      <c r="F399" s="16"/>
+      <c r="G399" s="16"/>
+      <c r="H399" s="18"/>
+      <c r="I399" s="19"/>
+      <c r="J399" s="16"/>
+      <c r="K399" s="16"/>
+      <c r="L399" s="18"/>
+      <c r="M399" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="400">
+      <c r="B400" s="0"/>
+      <c r="C400" s="31"/>
+      <c r="D400" s="32"/>
+      <c r="E400" s="32"/>
+      <c r="F400" s="16"/>
+      <c r="G400" s="16"/>
+      <c r="H400" s="18"/>
+      <c r="I400" s="19"/>
+      <c r="J400" s="16"/>
+      <c r="K400" s="16"/>
+      <c r="L400" s="18"/>
+      <c r="M400" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="401">
+      <c r="B401" s="0"/>
+      <c r="C401" s="31"/>
+      <c r="D401" s="32"/>
+      <c r="E401" s="32"/>
+      <c r="F401" s="16"/>
+      <c r="G401" s="16"/>
+      <c r="H401" s="18"/>
+      <c r="I401" s="19"/>
+      <c r="J401" s="16"/>
+      <c r="K401" s="16"/>
+      <c r="L401" s="18"/>
+      <c r="M401" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="402">
+      <c r="B402" s="0"/>
+      <c r="C402" s="31"/>
+      <c r="D402" s="32"/>
+      <c r="E402" s="32"/>
+      <c r="F402" s="16"/>
+      <c r="G402" s="16"/>
+      <c r="H402" s="18"/>
+      <c r="I402" s="19"/>
+      <c r="J402" s="16"/>
+      <c r="K402" s="16"/>
+      <c r="L402" s="18"/>
+      <c r="M402" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="403">
+      <c r="B403" s="0"/>
+      <c r="C403" s="31"/>
+      <c r="D403" s="32"/>
+      <c r="E403" s="32"/>
+      <c r="F403" s="16"/>
+      <c r="G403" s="16"/>
+      <c r="H403" s="18"/>
+      <c r="I403" s="19"/>
+      <c r="J403" s="16"/>
+      <c r="K403" s="16"/>
+      <c r="L403" s="18"/>
+      <c r="M403" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="404">
+      <c r="B404" s="30"/>
+      <c r="C404" s="31"/>
+      <c r="D404" s="32"/>
+      <c r="E404" s="32"/>
+      <c r="F404" s="16"/>
+      <c r="G404" s="16"/>
+      <c r="H404" s="18"/>
+      <c r="I404" s="19"/>
+      <c r="J404" s="16"/>
+      <c r="K404" s="16"/>
+      <c r="L404" s="18"/>
+      <c r="M404" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="405">
+      <c r="B405" s="30"/>
+      <c r="C405" s="31"/>
+      <c r="D405" s="32"/>
+      <c r="E405" s="32"/>
+      <c r="F405" s="16"/>
+      <c r="G405" s="16"/>
+      <c r="H405" s="18"/>
+      <c r="I405" s="19"/>
+      <c r="J405" s="16"/>
+      <c r="K405" s="16"/>
+      <c r="L405" s="18"/>
+      <c r="M405" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="406">
+      <c r="B406" s="30"/>
+      <c r="C406" s="31"/>
+      <c r="D406" s="32"/>
+      <c r="E406" s="32"/>
+      <c r="F406" s="16"/>
+      <c r="G406" s="16"/>
+      <c r="H406" s="18"/>
+      <c r="I406" s="19"/>
+      <c r="J406" s="16"/>
+      <c r="K406" s="16"/>
+      <c r="L406" s="18"/>
+      <c r="M406" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="407">
+      <c r="B407" s="30"/>
+      <c r="C407" s="31"/>
+      <c r="D407" s="32"/>
+      <c r="E407" s="32"/>
+      <c r="F407" s="16"/>
+      <c r="G407" s="16"/>
+      <c r="H407" s="18"/>
+      <c r="I407" s="19"/>
+      <c r="J407" s="16"/>
+      <c r="K407" s="16"/>
+      <c r="L407" s="18"/>
+      <c r="M407" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="408">
+      <c r="B408" s="30"/>
+      <c r="C408" s="31"/>
+      <c r="D408" s="32"/>
+      <c r="E408" s="32"/>
+      <c r="F408" s="16"/>
+      <c r="G408" s="16"/>
+      <c r="H408" s="18"/>
+      <c r="I408" s="19"/>
+      <c r="J408" s="16"/>
+      <c r="K408" s="16"/>
+      <c r="L408" s="18"/>
+      <c r="M408" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="409">
+      <c r="B409" s="30"/>
+      <c r="C409" s="31"/>
+      <c r="D409" s="32"/>
+      <c r="E409" s="32"/>
+      <c r="F409" s="16"/>
+      <c r="G409" s="16"/>
+      <c r="H409" s="18"/>
+      <c r="I409" s="19"/>
+      <c r="J409" s="16"/>
+      <c r="K409" s="16"/>
+      <c r="L409" s="18"/>
+      <c r="M409" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="410" s="66">
+      <c r="A410" s="64"/>
+      <c r="B410" s="30"/>
+      <c r="C410" s="31"/>
+      <c r="D410" s="32"/>
+      <c r="E410" s="32"/>
+      <c r="F410" s="16"/>
+      <c r="G410" s="16"/>
+      <c r="H410" s="18"/>
+      <c r="I410" s="19"/>
+      <c r="J410" s="16"/>
+      <c r="K410" s="16"/>
+      <c r="L410" s="18"/>
+      <c r="M410" s="19"/>
+      <c r="N410" s="65"/>
+      <c r="O410" s="65"/>
+      <c r="P410" s="65"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="411">
+      <c r="B411" s="30"/>
+      <c r="C411" s="31"/>
+      <c r="D411" s="32"/>
+      <c r="E411" s="32"/>
+      <c r="F411" s="16"/>
+      <c r="G411" s="16"/>
+      <c r="H411" s="18"/>
+      <c r="I411" s="19"/>
+      <c r="J411" s="16"/>
+      <c r="K411" s="16"/>
+      <c r="L411" s="18"/>
+      <c r="M411" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.5" outlineLevel="0" r="412">
+      <c r="B412" s="30" t="s">
+        <v>489</v>
+      </c>
+      <c r="C412" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D412" s="32" t="s">
+        <v>490</v>
+      </c>
+      <c r="E412" s="32" t="s">
+        <v>491</v>
+      </c>
+      <c r="F412" s="16"/>
+      <c r="G412" s="16"/>
+      <c r="H412" s="18"/>
+      <c r="I412" s="19"/>
+      <c r="J412" s="16"/>
+      <c r="K412" s="16"/>
+      <c r="L412" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M412" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="413">
+      <c r="B413" s="30" t="s">
+        <v>492</v>
+      </c>
+      <c r="C413" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D413" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="E413" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="F413" s="16"/>
+      <c r="G413" s="16"/>
+      <c r="H413" s="18"/>
+      <c r="I413" s="19"/>
+      <c r="J413" s="16"/>
+      <c r="K413" s="16"/>
+      <c r="L413" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M413" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.5" outlineLevel="0" r="414">
+      <c r="B414" s="30" t="s">
+        <v>493</v>
+      </c>
+      <c r="C414" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D414" s="32" t="s">
+        <v>490</v>
+      </c>
+      <c r="E414" s="32" t="s">
+        <v>491</v>
+      </c>
+      <c r="F414" s="16"/>
+      <c r="G414" s="16"/>
+      <c r="H414" s="18"/>
+      <c r="I414" s="19"/>
+      <c r="J414" s="16"/>
+      <c r="K414" s="16"/>
+      <c r="L414" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M414" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="415">
+      <c r="B415" s="30" t="s">
+        <v>494</v>
+      </c>
+      <c r="C415" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D415" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="E415" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="F415" s="16"/>
+      <c r="G415" s="16"/>
+      <c r="H415" s="18"/>
+      <c r="I415" s="19"/>
+      <c r="J415" s="16"/>
+      <c r="K415" s="16"/>
+      <c r="L415" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M415" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="49.5" outlineLevel="0" r="416">
+      <c r="B416" s="30" t="s">
+        <v>495</v>
+      </c>
+      <c r="C416" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D416" s="32" t="s">
+        <v>490</v>
+      </c>
+      <c r="E416" s="32" t="s">
+        <v>491</v>
+      </c>
+      <c r="F416" s="16"/>
+      <c r="G416" s="16"/>
+      <c r="H416" s="18"/>
+      <c r="I416" s="19"/>
+      <c r="J416" s="16"/>
+      <c r="K416" s="16"/>
+      <c r="L416" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M416" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="103.6" outlineLevel="0" r="417">
+      <c r="B417" s="30" t="s">
+        <v>496</v>
+      </c>
+      <c r="C417" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D417" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="E417" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="F417" s="16"/>
+      <c r="G417" s="16"/>
+      <c r="H417" s="18"/>
+      <c r="I417" s="19"/>
+      <c r="J417" s="16"/>
+      <c r="K417" s="16"/>
+      <c r="L417" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M417" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="103.6" outlineLevel="0" r="418">
+      <c r="B418" s="30"/>
+      <c r="C418" s="31"/>
+      <c r="D418" s="32"/>
+      <c r="E418" s="32"/>
+      <c r="F418" s="16"/>
+      <c r="G418" s="16"/>
+      <c r="H418" s="18"/>
+      <c r="I418" s="19"/>
+      <c r="J418" s="16"/>
+      <c r="K418" s="16"/>
+      <c r="L418" s="18"/>
+      <c r="M418" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="419">
+      <c r="B419" s="30" t="s">
+        <v>497</v>
+      </c>
+      <c r="C419" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D419" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="E419" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="F419" s="16"/>
+      <c r="G419" s="16"/>
+      <c r="H419" s="18"/>
+      <c r="I419" s="19"/>
+      <c r="J419" s="16"/>
+      <c r="K419" s="16"/>
+      <c r="L419" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M419" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="53.25" outlineLevel="0" r="420">
+      <c r="B420" s="30" t="s">
+        <v>498</v>
+      </c>
+      <c r="C420" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D420" s="32" t="s">
+        <v>490</v>
+      </c>
+      <c r="E420" s="32" t="s">
+        <v>491</v>
+      </c>
+      <c r="F420" s="16"/>
+      <c r="G420" s="16"/>
+      <c r="H420" s="18"/>
+      <c r="I420" s="19"/>
+      <c r="J420" s="16"/>
+      <c r="K420" s="16"/>
+      <c r="L420" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M420" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="54" outlineLevel="0" r="421">
+      <c r="B421" s="30" t="s">
+        <v>499</v>
+      </c>
+      <c r="C421" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D421" s="32" t="s">
+        <v>500</v>
+      </c>
+      <c r="E421" s="32" t="s">
+        <v>501</v>
+      </c>
+      <c r="F421" s="16"/>
+      <c r="G421" s="16"/>
+      <c r="H421" s="18"/>
+      <c r="I421" s="19"/>
+      <c r="J421" s="16"/>
+      <c r="K421" s="16"/>
+      <c r="L421" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M421" s="19" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="422">
+      <c r="A422" s="22"/>
+      <c r="B422" s="23"/>
+      <c r="C422" s="23"/>
+      <c r="D422" s="23"/>
+      <c r="E422" s="24"/>
+      <c r="F422" s="60"/>
+      <c r="G422" s="60"/>
+      <c r="H422" s="61"/>
+      <c r="I422" s="62"/>
+      <c r="J422" s="60"/>
+      <c r="K422" s="60"/>
+      <c r="L422" s="61"/>
+      <c r="M422" s="62"/>
+      <c r="N422" s="28"/>
+      <c r="O422" s="28"/>
+      <c r="P422" s="28"/>
+      <c r="Q422" s="28"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="423">
+      <c r="B423" s="15" t="s">
+        <v>502</v>
+      </c>
+      <c r="F423" s="16"/>
+      <c r="G423" s="16"/>
+      <c r="H423" s="18"/>
+      <c r="I423" s="19"/>
+      <c r="J423" s="16"/>
+      <c r="K423" s="16"/>
+      <c r="L423" s="18"/>
+      <c r="M423" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="424">
+      <c r="B424" s="30" t="s">
+        <v>503</v>
+      </c>
+      <c r="C424" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D424" s="32" t="s">
+        <v>504</v>
+      </c>
+      <c r="E424" s="32" t="s">
+        <v>505</v>
+      </c>
+      <c r="F424" s="16"/>
+      <c r="G424" s="16"/>
+      <c r="H424" s="18"/>
+      <c r="I424" s="19" t="s">
+        <v>506</v>
+      </c>
+      <c r="J424" s="16"/>
+      <c r="K424" s="16"/>
+      <c r="L424" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M424" s="19" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="425">
+      <c r="B425" s="30" t="s">
+        <v>507</v>
+      </c>
+      <c r="C425" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D425" s="32" t="s">
+        <v>508</v>
+      </c>
+      <c r="E425" s="32" t="s">
+        <v>509</v>
+      </c>
+      <c r="F425" s="16"/>
+      <c r="G425" s="16"/>
+      <c r="H425" s="18"/>
+      <c r="I425" s="19" t="s">
+        <v>506</v>
+      </c>
+      <c r="J425" s="16"/>
+      <c r="K425" s="16"/>
+      <c r="L425" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M425" s="19" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="426">
+      <c r="B426" s="30" t="s">
+        <v>510</v>
+      </c>
+      <c r="C426" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D426" s="32" t="s">
+        <v>511</v>
+      </c>
+      <c r="E426" s="32" t="s">
+        <v>512</v>
+      </c>
+      <c r="F426" s="16"/>
+      <c r="G426" s="16"/>
+      <c r="H426" s="18"/>
+      <c r="I426" s="19" t="s">
+        <v>506</v>
+      </c>
+      <c r="J426" s="16"/>
+      <c r="K426" s="16"/>
+      <c r="L426" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M426" s="19" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="427">
+      <c r="B427" s="30" t="s">
+        <v>513</v>
+      </c>
+      <c r="C427" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D427" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="E427" s="32" t="s">
+        <v>515</v>
+      </c>
+      <c r="F427" s="16"/>
+      <c r="G427" s="16"/>
+      <c r="H427" s="18"/>
+      <c r="I427" s="19" t="s">
+        <v>506</v>
+      </c>
+      <c r="J427" s="16"/>
+      <c r="K427" s="16"/>
+      <c r="L427" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M427" s="19" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="428">
+      <c r="B428" s="30" t="s">
+        <v>516</v>
+      </c>
+      <c r="C428" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D428" s="32" t="s">
+        <v>517</v>
+      </c>
+      <c r="E428" s="32" t="s">
+        <v>518</v>
+      </c>
+      <c r="F428" s="16"/>
+      <c r="G428" s="16"/>
+      <c r="H428" s="18"/>
+      <c r="I428" s="19" t="s">
+        <v>506</v>
+      </c>
+      <c r="J428" s="16"/>
+      <c r="K428" s="16"/>
+      <c r="L428" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M428" s="19" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="429">
+      <c r="B429" s="30" t="s">
+        <v>519</v>
+      </c>
+      <c r="C429" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D429" s="32" t="s">
+        <v>520</v>
+      </c>
+      <c r="E429" s="32" t="s">
+        <v>521</v>
+      </c>
+      <c r="F429" s="16"/>
+      <c r="G429" s="16"/>
+      <c r="H429" s="18"/>
+      <c r="I429" s="19" t="s">
+        <v>506</v>
+      </c>
+      <c r="J429" s="16"/>
+      <c r="K429" s="16"/>
+      <c r="L429" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M429" s="19" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="60" outlineLevel="0" r="430">
+      <c r="B430" s="30" t="s">
+        <v>522</v>
+      </c>
+      <c r="C430" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D430" s="32" t="s">
+        <v>523</v>
+      </c>
+      <c r="E430" s="32" t="s">
+        <v>524</v>
+      </c>
+      <c r="F430" s="16"/>
+      <c r="G430" s="16"/>
+      <c r="H430" s="18"/>
+      <c r="I430" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="J430" s="16"/>
+      <c r="K430" s="16"/>
+      <c r="L430" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M430" s="35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45" outlineLevel="0" r="431">
+      <c r="B431" s="30" t="s">
+        <v>525</v>
+      </c>
+      <c r="C431" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D431" s="32" t="s">
+        <v>526</v>
+      </c>
+      <c r="E431" s="32" t="s">
+        <v>527</v>
+      </c>
+      <c r="F431" s="16"/>
+      <c r="G431" s="16"/>
+      <c r="H431" s="18"/>
+      <c r="I431" s="19" t="s">
+        <v>528</v>
+      </c>
+      <c r="J431" s="16"/>
+      <c r="K431" s="16"/>
+      <c r="L431" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M431" s="19" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="45.75" outlineLevel="0" r="432">
+      <c r="B432" s="30" t="s">
+        <v>529</v>
+      </c>
+      <c r="C432" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D432" s="32" t="s">
+        <v>530</v>
+      </c>
+      <c r="E432" s="32" t="s">
+        <v>531</v>
+      </c>
+      <c r="F432" s="16"/>
+      <c r="G432" s="16"/>
+      <c r="H432" s="18"/>
+      <c r="I432" s="19" t="s">
+        <v>528</v>
+      </c>
+      <c r="J432" s="16"/>
+      <c r="K432" s="16"/>
+      <c r="L432" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M432" s="19" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="433">
+      <c r="A433" s="22"/>
+      <c r="B433" s="23"/>
+      <c r="C433" s="23"/>
+      <c r="D433" s="23"/>
+      <c r="E433" s="24"/>
+      <c r="F433" s="60"/>
+      <c r="G433" s="60"/>
+      <c r="H433" s="61"/>
+      <c r="I433" s="62"/>
+      <c r="J433" s="60"/>
+      <c r="K433" s="60"/>
+      <c r="L433" s="61"/>
+      <c r="M433" s="62"/>
+      <c r="N433" s="28"/>
+      <c r="O433" s="28"/>
+      <c r="P433" s="28"/>
+      <c r="Q433" s="28"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="434">
+      <c r="B434" s="15" t="s">
+        <v>532</v>
+      </c>
+      <c r="F434" s="16"/>
+      <c r="G434" s="16"/>
+      <c r="H434" s="18"/>
+      <c r="I434" s="19"/>
+      <c r="J434" s="16"/>
+      <c r="K434" s="16"/>
+      <c r="L434" s="18"/>
+      <c r="M434" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="19.2" outlineLevel="0" r="435" s="43">
+      <c r="A435" s="39"/>
+      <c r="B435" s="49" t="s">
+        <v>533</v>
+      </c>
+      <c r="C435" s="31"/>
+      <c r="D435" s="20"/>
+      <c r="E435" s="20"/>
+      <c r="F435" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G435" s="51" t="inlineStr">
+        <f aca="true">NOW()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H435" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="I435" s="42" t="s">
+        <v>534</v>
+      </c>
+      <c r="J435" s="40"/>
+      <c r="K435" s="40"/>
+      <c r="L435" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="M435" s="42" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24.85" outlineLevel="0" r="436" s="43">
+      <c r="A436" s="39"/>
+      <c r="B436" s="49" t="s">
+        <v>535</v>
+      </c>
+      <c r="C436" s="31"/>
+      <c r="D436" s="20"/>
+      <c r="E436" s="20"/>
+      <c r="F436" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G436" s="51" t="inlineStr">
+        <f aca="true">NOW()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H436" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="I436" s="42"/>
+      <c r="J436" s="40"/>
+      <c r="K436" s="40"/>
+      <c r="L436" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="M436" s="42"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="36.15" outlineLevel="0" r="437" s="43">
+      <c r="A437" s="39"/>
+      <c r="B437" s="49" t="s">
+        <v>536</v>
+      </c>
+      <c r="C437" s="31"/>
+      <c r="D437" s="20"/>
+      <c r="E437" s="20"/>
+      <c r="F437" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G437" s="51" t="inlineStr">
+        <f aca="true">NOW()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H437" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I437" s="42"/>
+      <c r="J437" s="40"/>
+      <c r="K437" s="40"/>
+      <c r="L437" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="M437" s="42" t="s">
+        <v>537</v>
+      </c>
+      <c r="N437" s="43" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30.75" outlineLevel="0" r="438" s="43">
+      <c r="A438" s="39"/>
+      <c r="B438" s="49" t="s">
+        <v>538</v>
+      </c>
+      <c r="C438" s="31"/>
+      <c r="D438" s="20"/>
+      <c r="E438" s="20"/>
+      <c r="F438" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G438" s="51" t="inlineStr">
+        <f aca="true">NOW()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H438" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="I438" s="42" t="s">
+        <v>539</v>
+      </c>
+      <c r="J438" s="40"/>
+      <c r="K438" s="40"/>
+      <c r="L438" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="M438" s="42" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="439">
+      <c r="A439" s="22"/>
+      <c r="B439" s="23"/>
+      <c r="C439" s="23"/>
+      <c r="D439" s="23"/>
+      <c r="E439" s="24"/>
+      <c r="F439" s="60"/>
+      <c r="G439" s="60"/>
+      <c r="H439" s="61"/>
+      <c r="I439" s="62"/>
+      <c r="J439" s="60"/>
+      <c r="K439" s="60"/>
+      <c r="L439" s="61"/>
+      <c r="M439" s="62"/>
+      <c r="N439" s="28"/>
+      <c r="O439" s="28"/>
+      <c r="P439" s="28"/>
+      <c r="Q439" s="28"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="440">
+      <c r="B440" s="15" t="s">
+        <v>540</v>
+      </c>
+      <c r="F440" s="16"/>
+      <c r="G440" s="16"/>
+      <c r="H440" s="18"/>
+      <c r="I440" s="19"/>
+      <c r="J440" s="16"/>
+      <c r="K440" s="16"/>
+      <c r="L440" s="18"/>
+      <c r="M440" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="441" s="43">
+      <c r="A441" s="50"/>
+      <c r="B441" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="C441" s="58" t="s">
+        <v>279</v>
+      </c>
+      <c r="D441" s="20"/>
+      <c r="E441" s="20"/>
+      <c r="F441" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G441" s="51" t="inlineStr">
+        <f aca="true">NOW()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H441" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="I441" s="42" t="s">
+        <v>542</v>
+      </c>
+      <c r="J441" s="40"/>
+      <c r="K441" s="40"/>
+      <c r="L441" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="M441" s="42"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="442" s="43">
+      <c r="A442" s="50"/>
+      <c r="B442" s="56" t="s">
+        <v>543</v>
+      </c>
+      <c r="C442" s="58" t="s">
+        <v>279</v>
+      </c>
+      <c r="D442" s="20"/>
+      <c r="E442" s="20"/>
+      <c r="F442" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G442" s="51" t="inlineStr">
+        <f aca="true">NOW()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H442" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="I442" s="42" t="s">
+        <v>542</v>
+      </c>
+      <c r="J442" s="40"/>
+      <c r="K442" s="40"/>
+      <c r="L442" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="M442" s="42"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="443" s="43">
+      <c r="A443" s="50"/>
+      <c r="B443" s="56" t="s">
+        <v>544</v>
+      </c>
+      <c r="C443" s="58" t="s">
+        <v>279</v>
+      </c>
+      <c r="D443" s="20"/>
+      <c r="E443" s="20"/>
+      <c r="F443" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G443" s="51" t="inlineStr">
+        <f aca="true">NOW()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H443" s="52" t="n">
+        <v>9</v>
+      </c>
+      <c r="I443" s="42"/>
+      <c r="J443" s="40"/>
+      <c r="K443" s="40"/>
+      <c r="L443" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="M443" s="42" t="s">
+        <v>545</v>
+      </c>
+      <c r="N443" s="43" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="44.05" outlineLevel="0" r="444" s="43">
+      <c r="A444" s="50"/>
+      <c r="B444" s="56" t="s">
+        <v>546</v>
+      </c>
+      <c r="C444" s="58" t="s">
+        <v>279</v>
+      </c>
+      <c r="D444" s="20"/>
+      <c r="E444" s="20"/>
+      <c r="F444" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G444" s="51" t="inlineStr">
+        <f aca="true">NOW()</f>
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H444" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I444" s="42" t="s">
+        <v>547</v>
+      </c>
+      <c r="J444" s="40"/>
+      <c r="K444" s="40"/>
+      <c r="L444" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="M444" s="42"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="30" outlineLevel="0" r="445" s="43">
+      <c r="A445" s="50"/>
+      <c r="B445" s="56" t="s">
+        <v>548</v>
+      </c>
+      <c r="C445" s="58" t="s">
+        <v>279</v>
+      </c>
+      <c r="D445" s="20"/>
+      <c r="E445" s="20"/>
+      <c r="F445" s="40"/>
+      <c r="G445" s="40"/>
+      <c r="H445" s="52"/>
+      <c r="I445" s="42"/>
+      <c r="J445" s="40"/>
+      <c r="K445" s="40"/>
+      <c r="L445" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="M445" s="42"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="446">
+      <c r="F446" s="16"/>
+      <c r="G446" s="16"/>
+      <c r="H446" s="18"/>
+      <c r="I446" s="19"/>
+      <c r="J446" s="16"/>
+      <c r="K446" s="16"/>
+      <c r="L446" s="18"/>
+      <c r="M446" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="447">
+      <c r="F447" s="16"/>
+      <c r="G447" s="16"/>
+      <c r="H447" s="18"/>
+      <c r="I447" s="19"/>
+      <c r="J447" s="16"/>
+      <c r="K447" s="16"/>
+      <c r="L447" s="18"/>
+      <c r="M447" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="448">
+      <c r="F448" s="16"/>
+      <c r="G448" s="16"/>
+      <c r="H448" s="18"/>
+      <c r="I448" s="19"/>
+      <c r="J448" s="16"/>
+      <c r="K448" s="16"/>
+      <c r="L448" s="18"/>
+      <c r="M448" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.75" outlineLevel="0" r="449">
+      <c r="F449" s="16"/>
+      <c r="G449" s="16"/>
+      <c r="H449" s="18"/>
+      <c r="I449" s="19"/>
+      <c r="J449" s="16"/>
+      <c r="K449" s="16"/>
+      <c r="L449" s="18"/>
+      <c r="M449" s="19"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="450">
+      <c r="A450" s="22"/>
+      <c r="B450" s="23"/>
+      <c r="C450" s="23"/>
+      <c r="D450" s="23"/>
+      <c r="E450" s="23"/>
+      <c r="F450" s="67"/>
+      <c r="G450" s="67"/>
+      <c r="H450" s="26"/>
+      <c r="I450" s="27"/>
+      <c r="J450" s="67"/>
+      <c r="K450" s="67"/>
+      <c r="L450" s="26"/>
+      <c r="M450" s="27"/>
+      <c r="N450" s="28"/>
+      <c r="O450" s="28"/>
+      <c r="P450" s="28"/>
+      <c r="Q450" s="28"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="451">
+      <c r="A451" s="22"/>
+      <c r="B451" s="23"/>
+      <c r="C451" s="23"/>
+      <c r="D451" s="23"/>
+      <c r="E451" s="23"/>
+      <c r="F451" s="68"/>
+      <c r="G451" s="68"/>
+      <c r="H451" s="69"/>
+      <c r="I451" s="27"/>
+      <c r="J451" s="68"/>
+      <c r="K451" s="68"/>
+      <c r="L451" s="69"/>
+      <c r="M451" s="27"/>
+      <c r="N451" s="28"/>
+      <c r="O451" s="28"/>
+      <c r="P451" s="28"/>
+      <c r="Q451" s="28"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="452">
+      <c r="A452" s="22"/>
+      <c r="B452" s="23"/>
+      <c r="C452" s="23"/>
+      <c r="D452" s="23"/>
+      <c r="E452" s="23"/>
+      <c r="F452" s="68"/>
+      <c r="G452" s="68"/>
+      <c r="H452" s="69"/>
+      <c r="I452" s="27"/>
+      <c r="J452" s="68"/>
+      <c r="K452" s="68"/>
+      <c r="L452" s="69"/>
+      <c r="M452" s="27"/>
+      <c r="N452" s="28"/>
+      <c r="O452" s="28"/>
+      <c r="P452" s="28"/>
+      <c r="Q452" s="28"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="453">
+      <c r="A453" s="22"/>
+      <c r="B453" s="23"/>
+      <c r="C453" s="23"/>
+      <c r="D453" s="23"/>
+      <c r="E453" s="23"/>
+      <c r="F453" s="68"/>
+      <c r="G453" s="68"/>
+      <c r="H453" s="69"/>
+      <c r="I453" s="27"/>
+      <c r="J453" s="68"/>
+      <c r="K453" s="68"/>
+      <c r="L453" s="69"/>
+      <c r="M453" s="27"/>
+      <c r="N453" s="28"/>
+      <c r="O453" s="28"/>
+      <c r="P453" s="28"/>
+      <c r="Q453" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>